<commit_message>
fix: test cases of Book Catalog module is complete
</commit_message>
<xml_diff>
--- a/test_cases/Book Catalog - Test Cases.xlsx
+++ b/test_cases/Book Catalog - Test Cases.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\PROGRAMMING_HABIT\bookcatalog-automation\test_cases\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2AFEB6D6-57FB-41F0-986B-490B4C0D4142}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{20C8B178-147E-47BC-AD88-CF34C9AB92A2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Title" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="197" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="342" uniqueCount="203">
   <si>
     <t>Application name</t>
   </si>
@@ -231,9 +231,6 @@
     <t>Ship</t>
   </si>
   <si>
-    <t>Stone</t>
-  </si>
-  <si>
     <t>Delete functionality</t>
   </si>
   <si>
@@ -241,9 +238,6 @@
   </si>
   <si>
     <t>Data table next/previous functionality</t>
-  </si>
-  <si>
-    <t>Verify if user is able to add new book with empty forms and select category selected</t>
   </si>
   <si>
     <t>1. Go to http://localhost/bookcatalog/views/bookcatalog.php
@@ -255,30 +249,6 @@
   </si>
   <si>
     <t>User see the validation modal and message and unable to add new book.</t>
-  </si>
-  <si>
-    <t>Verify if user is able to add new book 
-with empty Title</t>
-  </si>
-  <si>
-    <t>Verify if user is able to add new book 
-with empty ISBN</t>
-  </si>
-  <si>
-    <t>Verify if user is able to add new book
-with empty Author</t>
-  </si>
-  <si>
-    <t>Verify if user is able to add new book
-with empty Publisher</t>
-  </si>
-  <si>
-    <t>Verify if user is able to add new book
-with unselected category</t>
-  </si>
-  <si>
-    <t>Verify if user is able to add new book
-with filled-in forms and selected category</t>
   </si>
   <si>
     <t>1. Go to http://localhost/bookcatalog/views/bookcatalog.php
@@ -348,12 +318,610 @@
     <t>User able to add new book and see the modal with 
 message of "Successfully add new book!".</t>
   </si>
+  <si>
+    <t>1. Go to http://localhost/bookcatalog/views/bookcatalog.php
+2. Click ADD green button
+3. Click Back gray button</t>
+  </si>
+  <si>
+    <t>User should be able to go back once add modal pop-up.</t>
+  </si>
+  <si>
+    <t>User is able to go back by clicking back once add modal pop-up.</t>
+  </si>
+  <si>
+    <t>1. Go to http://localhost/bookcatalog/views/bookcatalog.php
+2. Click ADD green button
+3. Enter Title (The Titan's Curse)
+4. Enter ISBN (5)
+5. Enter Author (Rick Riordan)
+6. Enter Publisher (Manila Times)
+7. Select Fiction category
+8. Click Back gray button
+9. Click ADD green button</t>
+  </si>
+  <si>
+    <t>User should be able to fill-in forms and select category, also able to go back by clicking Back gray button on add modal. Once the user click the ADD green button again, the forms should be empty and unselect category.</t>
+  </si>
+  <si>
+    <t>User is able to fill-in forms and select category, can also go back by clicking Back gray button. By re-clicking the ADD green button, user able to see empty forms and unselected category.</t>
+  </si>
+  <si>
+    <t>Verify if user is able to edit book details with empty forms and unselected category</t>
+  </si>
+  <si>
+    <t>1. Go to http://localhost/bookcatalog/views/bookcatalog.php
+2. Click Edit gray button
+3. Clear Title details
+4. Clear ISBN details
+5. Clear Author details
+6. Clear Publisher details
+7. Unselect category (Select category)
+8. Click Update blue button</t>
+  </si>
+  <si>
+    <t>User should see the validation modal and message "Please fill-up everything." and will not be able to edit book details with empty forms.</t>
+  </si>
+  <si>
+    <t>User see the validation modal and message and unable to edit book details.</t>
+  </si>
+  <si>
+    <t>1. Go to http://localhost/bookcatalog/views/bookcatalog.php
+2. Check details of book that is about to edit details.
+3. Click Edit gray button</t>
+  </si>
+  <si>
+    <t>Verify if the user is able to get the correct details from the book that was selected for editing.</t>
+  </si>
+  <si>
+    <t>The user should be able to see the edit modal with the correct details from the book that was selected for editing.</t>
+  </si>
+  <si>
+    <t>The user sees the edit modal pop up with the correct details.</t>
+  </si>
+  <si>
+    <t>Verify if user is able to go back by clicking back button after clicking the Edit gray button.</t>
+  </si>
+  <si>
+    <t>1. Go to http://localhost/bookcatalog/views/bookcatalog.php
+2. Click Edit gray button
+8. Click Back gray button
+9. Click Edit gray button</t>
+  </si>
+  <si>
+    <t>User should be able to see edit modal pop up with correct details, also able to go back by clicking Back gray button on edit modal. Once the user click the Edit gray button again, the forms should be with the same details and selected category.</t>
+  </si>
+  <si>
+    <t>User is able to see edit modal pop up with correct details, can also go back by clicking Back gray button. By re-clicking the Edit gray button, user able to see correct details and selected category.</t>
+  </si>
+  <si>
+    <t>Verify if user is able to edit book details 
+with empty Title.</t>
+  </si>
+  <si>
+    <t>1. Go to http://localhost/bookcatalog/views/bookcatalog.php
+2. Click Edit gray button
+3. Erase Title details
+4. Click Update blue button</t>
+  </si>
+  <si>
+    <t>1. Go to http://localhost/bookcatalog/views/bookcatalog.php
+2. Click Edit gray button
+3. Erase ISBN details
+4. Click Update blue button</t>
+  </si>
+  <si>
+    <t>1. Go to http://localhost/bookcatalog/views/bookcatalog.php
+2. Click Edit gray button
+3. Erase Author details
+4. Click Update blue button</t>
+  </si>
+  <si>
+    <t>1. Go to http://localhost/bookcatalog/views/bookcatalog.php
+2. Click Edit gray button
+3. Erase Publisher details
+4. Click Update blue button</t>
+  </si>
+  <si>
+    <t>1. Go to http://localhost/bookcatalog/views/bookcatalog.php
+2. Click Edit gray button
+3. Select (Select category)
+4. Click Update blue button</t>
+  </si>
+  <si>
+    <t>Verify if user is unable to edit book 
+details with empty ISBN.</t>
+  </si>
+  <si>
+    <t>Verify if user is unable to edit book 
+details with empty Author.</t>
+  </si>
+  <si>
+    <t>Verify if user is unable to edit book 
+details with empty Publisher.</t>
+  </si>
+  <si>
+    <t>Verify if user is unable to edit book 
+details with unselected category.</t>
+  </si>
+  <si>
+    <t>Verify if user is able to go back to Add modal after clicking the Ok button on validation modal.</t>
+  </si>
+  <si>
+    <t>User should see the validation modal and message "Please fill-up everything." and able to go back to Add modal after clicking the Ok gray button.</t>
+  </si>
+  <si>
+    <t>User sees the validation modal and message "Please fill-up everything." and able to go back to Add modal after clicking the Ok gray button.</t>
+  </si>
+  <si>
+    <t>Verify if user is able to go back to Edit modal after clicking the Ok button on validation modal.</t>
+  </si>
+  <si>
+    <t>User should see the validation modal and message "Please fill-up everything." and able to go back to Edit modal after clicking the Ok gray button.</t>
+  </si>
+  <si>
+    <t>User sees the validation modal and message "Please fill-up everything." and able to go back to Edit modal after clicking the Ok gray button.</t>
+  </si>
+  <si>
+    <t>Verify if user is able to edit book details
+with filled-in forms and selected category</t>
+  </si>
+  <si>
+    <t>1. Go to http://localhost/bookcatalog/views/bookcatalog.php
+2. Click ADD green button
+3. Enter Title (Chamber of Secrets)
+4. Enter ISBN (13)
+5. Enter Author (Rick Riordan)
+6. Enter Publisher (Manila Times)
+7. Select Fiction category
+8. Click Update blue button</t>
+  </si>
+  <si>
+    <t>1. Go to http://localhost/bookcatalog/views/bookcatalog.php
+2. Click ADD green button
+3. Enter Title (The Titan's Curse)
+4. Enter ISBN (5)
+5. Enter Author (Rick Riordan)
+6. Enter Publisher (Manila Times)
+7. Unselect category (Select category)
+8. Click Update blue button</t>
+  </si>
+  <si>
+    <t>User should be able to edit book details and 
+see the modal with the message of "Update details successfully!".</t>
+  </si>
+  <si>
+    <t>User able to edit book details and sees the modal with 
+message of "Update details successfully!".</t>
+  </si>
+  <si>
+    <t>Verify if user is unable to add new book with empty forms and select category selected</t>
+  </si>
+  <si>
+    <t>Verify if user is unable to add new book 
+with empty Title</t>
+  </si>
+  <si>
+    <t>Verify if user is unable to add new book 
+with empty ISBN</t>
+  </si>
+  <si>
+    <t>Verify if user is unable to add new book
+with empty Author</t>
+  </si>
+  <si>
+    <t>Verify if user is unable to add new book
+with empty Publisher</t>
+  </si>
+  <si>
+    <t>Verify if user is unable to add new book
+with unselected category</t>
+  </si>
+  <si>
+    <t>Verify if user is able to go back by clicking back button after clicking the Add green button.</t>
+  </si>
+  <si>
+    <t>Verify if user is able to add new book
+with filled-in forms and selected category.</t>
+  </si>
+  <si>
+    <t>Verify if user is able to see modal of 
+delete.</t>
+  </si>
+  <si>
+    <t>User should be able to see delete modal with the
+ message of "Are you sure to delete this book?".</t>
+  </si>
+  <si>
+    <t>User able to see delete modal with such message 
+"Are you sure to delete this book?".</t>
+  </si>
+  <si>
+    <t>1. Go to http://localhost/bookcatalog/views/bookcatalog.php
+2. Click Delete red button</t>
+  </si>
+  <si>
+    <t>Verify if user is able to go back after 
+delete modal pop up.</t>
+  </si>
+  <si>
+    <t>1. Go to http://localhost/bookcatalog/views/bookcatalog.php
+2. Click Delete red button
+3. Click Back gray button</t>
+  </si>
+  <si>
+    <t>User should be able to go back after clicking the Back gray button 
+without deleting the book.</t>
+  </si>
+  <si>
+    <t>User is able to go back after clicking the Back gray button 
+without deleting the book.</t>
+  </si>
+  <si>
+    <t>Verify if user is able to delete book.</t>
+  </si>
+  <si>
+    <t>1. Go to http://localhost/bookcatalog/views/bookcatalog.php
+2. Click Delete red button (data table)
+3. Click Delete red button (modal)</t>
+  </si>
+  <si>
+    <t>User is able to delete book and sees the 
+message of "Delete successfully!" modal.</t>
+  </si>
+  <si>
+    <t>User should be able to delete book and see the 
+message of "Delete successfully!" modal.</t>
+  </si>
+  <si>
+    <t>Verify datatable if user click the 
+Active filter</t>
+  </si>
+  <si>
+    <t>Verify datatable if user click the 
+Deleted filter</t>
+  </si>
+  <si>
+    <t>Verify datatable if user click the 
+All filter</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Go to http://localhost/bookcatalog/views/bookcatalog.php
+2. Select Active </t>
+  </si>
+  <si>
+    <t>1. Go to http://localhost/bookcatalog/views/bookcatalog.php
+2. Select Deleted</t>
+  </si>
+  <si>
+    <t>1. Go to http://localhost/bookcatalog/views/bookcatalog.php
+2. Select All</t>
+  </si>
+  <si>
+    <t>User should be able to see the datatable with Edit and Delete 
+in ACTIONS column.</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">User should be able to see the datatable with </t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Deleted</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+in ACTIONS column.</t>
+    </r>
+  </si>
+  <si>
+    <t>User is able to see all the Edit and Delete in 
+datatables under ACTIONS column.</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">User is able to see all the </t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Deleted</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> in 
+datatables under ACTIONS column.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">User should be able to see the datatable with Edit and Delete, and </t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Deleted</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> category in ACTIONS column.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">User is able to see all the Edit and Delete, and </t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Deleted</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> categories in datatables under ACTIONS column.</t>
+    </r>
+  </si>
+  <si>
+    <t>Verify if user is able to search book 
+in search form.</t>
+  </si>
+  <si>
+    <t>1. Go to http://localhost/bookcatalog/views/bookcatalog.php
+2. Search "Phi" in search forms
+3. Click enter</t>
+  </si>
+  <si>
+    <t>1. Go to http://localhost/bookcatalog/views/bookcatalog.php
+2. Search "Cham" in search forms
+3. Click enter</t>
+  </si>
+  <si>
+    <t>1. Go to http://localhost/bookcatalog/views/bookcatalog.php
+2. Search "The" in search forms
+3. Click enter</t>
+  </si>
+  <si>
+    <t>1. Go to http://localhost/bookcatalog/views/bookcatalog.php
+2. Search "Highly" in search forms
+3. Click enter</t>
+  </si>
+  <si>
+    <t>1. Go to http://localhost/bookcatalog/views/bookcatalog.php
+2. Search "Ship" in search forms
+3. Click enter</t>
+  </si>
+  <si>
+    <t>qweqwewqewqe</t>
+  </si>
+  <si>
+    <t>1. Go to http://localhost/bookcatalog/views/bookcatalog.php
+2. Search "qweqwewqewqe" in search forms
+3. Click enter</t>
+  </si>
+  <si>
+    <t>Verify if user is able to click 
+number carousel in the datatable</t>
+  </si>
+  <si>
+    <t>Verify if user is able to click 
+next in the datatable</t>
+  </si>
+  <si>
+    <t>Verify if user is able to click 
+previous in the datatable</t>
+  </si>
+  <si>
+    <t>Verify if user is able to click 
+last in the datatable</t>
+  </si>
+  <si>
+    <t>Verify if user is able to click 
+current in the datatable</t>
+  </si>
+  <si>
+    <t>1. Go to http://localhost/bookcatalog/views/bookcatalog.php
+2. Click any number below the datatable</t>
+  </si>
+  <si>
+    <t>1. Go to http://localhost/bookcatalog/views/bookcatalog.php
+2. Click next (&gt;) below the datatable</t>
+  </si>
+  <si>
+    <t>1. Go to http://localhost/bookcatalog/views/bookcatalog.php
+2. Click previous (&lt;) below the datatable</t>
+  </si>
+  <si>
+    <t>1. Go to http://localhost/bookcatalog/views/bookcatalog.php
+2. Click last (&gt;&gt;) below the datatable</t>
+  </si>
+  <si>
+    <t>1. Go to http://localhost/bookcatalog/views/bookcatalog.php
+2. Click current (&lt;&lt;) below the datatable</t>
+  </si>
+  <si>
+    <t>User should see the message in the datatable,
+ "No data available in the table".</t>
+  </si>
+  <si>
+    <t>User is able to see the message 
+"No data available in the table".</t>
+  </si>
+  <si>
+    <t>User should be able to see all the book with the title of 
+atleast "Phi" or "phi" on it.</t>
+  </si>
+  <si>
+    <t>User should be able to see all the book with the title of 
+atleast "Cham" or "cham" on it.</t>
+  </si>
+  <si>
+    <t>User should be able to see all the book with the title of 
+atleast "The" or "the" on it.</t>
+  </si>
+  <si>
+    <t>User should be able to see all the book with the title of 
+atleast "Highly" or "highly" on it.</t>
+  </si>
+  <si>
+    <t>User should be able to see all the book with the title of 
+atleast "Ship" or "ship" on it.</t>
+  </si>
+  <si>
+    <t>User is able to see all the book list down on the datatable
+with the title of atleast "Phi" or "phi".</t>
+  </si>
+  <si>
+    <t>User is able to see all the book list down on the datatable
+with the title of atleast "The" or "the".</t>
+  </si>
+  <si>
+    <t>User is able to see all the book list down on the datatable
+with the title of atleast "Highly" or "highly".</t>
+  </si>
+  <si>
+    <t>User is able to see all the book list down on the datatable
+with the title of atleast "Cham" or "cham".</t>
+  </si>
+  <si>
+    <t>User is able to see all the book list down on the datatable
+with the title of atleast "Ship" or "ship".</t>
+  </si>
+  <si>
+    <t>User should be able to see all the books that belong
+to current number selected.</t>
+  </si>
+  <si>
+    <t>User should be able to see all the books that belong
+to previous list.</t>
+  </si>
+  <si>
+    <t>User should be able to see all the books that belong
+to next list.</t>
+  </si>
+  <si>
+    <t>User should be able to see all the books that belong
+to last list.</t>
+  </si>
+  <si>
+    <t>User is able to see the list of books in the selected number.</t>
+  </si>
+  <si>
+    <t>User is able to see the list of books in the next list.</t>
+  </si>
+  <si>
+    <t>User is able to see the list of books in the last list.</t>
+  </si>
+  <si>
+    <t>User is able to see the list of books in the previous list.</t>
+  </si>
+  <si>
+    <t>User is able to see the list of books in the current or first list.</t>
+  </si>
+  <si>
+    <t>User should be able to see all the books that belong
+to current or first list.</t>
+  </si>
+  <si>
+    <t>Verify if user is unable to add new book with string or not a number detail in the ISBN form.</t>
+  </si>
+  <si>
+    <t>1. Go to http://localhost/bookcatalog/views/bookcatalog.php
+2. Click ADD green button
+3. Enter Title (The Titan's Curse)
+4. Enter ISBN (BC-0005)
+5. Enter Author (Rick Riordan)
+6. Enter Publisher (Manila Times)
+7. Select Anime category
+8. Click Add blue button</t>
+  </si>
+  <si>
+    <t>User should not be able to add new book since the ISBN datatype is 
+number and should not accept string.</t>
+  </si>
+  <si>
+    <t>BUG</t>
+  </si>
+  <si>
+    <t>1. Go to http://localhost/bookcatalog/views/bookcatalog.php
+2. Click Edit gray button
+3. Enter "BC-0005" in the ISBN form.
+4. Click Update blue button</t>
+  </si>
+  <si>
+    <t>User should not be able to edit book detail since the ISBN datatype is 
+number and should not accept string.</t>
+  </si>
+  <si>
+    <t>User is able to edit book details and returns to 0 instead of "BC-0005".</t>
+  </si>
+  <si>
+    <t>User is able to add new book and returns to 0 instead of "BC-0005".</t>
+  </si>
+  <si>
+    <t>A- High</t>
+  </si>
+  <si>
+    <t>Please see screenshot id 1</t>
+  </si>
+  <si>
+    <t>Please see screenshot id 2</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -398,8 +966,16 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="9">
+  <fills count="11">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -445,6 +1021,18 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="8" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-4.9989318521683403E-2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -545,7 +1133,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -567,6 +1155,27 @@
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -574,6 +1183,9 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
@@ -591,21 +1203,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
@@ -615,14 +1212,23 @@
     <xf numFmtId="0" fontId="5" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="10" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -640,6 +1246,275 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>1</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>342901</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>174347</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="Picture 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{070CC366-FA5B-AE8E-11D6-6DA81EF380B9}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="838201" y="190500"/>
+          <a:ext cx="3371850" cy="2955647"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>256533</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>18843</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="5" name="Picture 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F5BECE05-8E7F-08C1-55B2-15182D0ED88E}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4476750" y="190500"/>
+          <a:ext cx="5133333" cy="1657143"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>33</xdr:col>
+      <xdr:colOff>446095</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>57033</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="6" name="Picture 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{32747F43-48E0-35F2-707D-10AC0AE6EFBB}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="9963150" y="190500"/>
+          <a:ext cx="12638095" cy="933333"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>333375</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>136599</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="7" name="Picture 6">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C13EB4C5-3542-004D-5ED3-6D58AD2F0B0E}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="838200" y="3352800"/>
+          <a:ext cx="3362325" cy="2994099"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>18438</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>180786</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="8" name="Picture 7">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{10E51846-F802-6005-DF7E-FA984C97F9CE}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4476750" y="3352800"/>
+          <a:ext cx="4895238" cy="1514286"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>33</xdr:col>
+      <xdr:colOff>446095</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>171333</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="9" name="Picture 8">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E6A732F6-56BD-4CCC-B356-94F2357CA5FE}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="9963150" y="3352800"/>
+          <a:ext cx="12638095" cy="933333"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -907,321 +1782,321 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z24"/>
   <sheetViews>
-    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="K15" sqref="K15:V15"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="I33" sqref="I33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="20" t="s">
+      <c r="A1" s="16" t="s">
         <v>29</v>
       </c>
-      <c r="B1" s="20"/>
-      <c r="C1" s="20"/>
-      <c r="D1" s="20"/>
-      <c r="E1" s="20"/>
-      <c r="F1" s="20"/>
-      <c r="G1" s="20"/>
-      <c r="H1" s="20"/>
-      <c r="I1" s="20"/>
-      <c r="J1" s="20"/>
-      <c r="K1" s="20"/>
-      <c r="L1" s="20"/>
-      <c r="M1" s="20"/>
-      <c r="N1" s="20"/>
-      <c r="O1" s="20"/>
-      <c r="P1" s="20"/>
-      <c r="Q1" s="20"/>
-      <c r="R1" s="20"/>
-      <c r="S1" s="20"/>
-      <c r="T1" s="20"/>
-      <c r="U1" s="20"/>
-      <c r="V1" s="20"/>
-      <c r="W1" s="20"/>
-      <c r="X1" s="20"/>
-      <c r="Y1" s="20"/>
-      <c r="Z1" s="20"/>
+      <c r="B1" s="16"/>
+      <c r="C1" s="16"/>
+      <c r="D1" s="16"/>
+      <c r="E1" s="16"/>
+      <c r="F1" s="16"/>
+      <c r="G1" s="16"/>
+      <c r="H1" s="16"/>
+      <c r="I1" s="16"/>
+      <c r="J1" s="16"/>
+      <c r="K1" s="16"/>
+      <c r="L1" s="16"/>
+      <c r="M1" s="16"/>
+      <c r="N1" s="16"/>
+      <c r="O1" s="16"/>
+      <c r="P1" s="16"/>
+      <c r="Q1" s="16"/>
+      <c r="R1" s="16"/>
+      <c r="S1" s="16"/>
+      <c r="T1" s="16"/>
+      <c r="U1" s="16"/>
+      <c r="V1" s="16"/>
+      <c r="W1" s="16"/>
+      <c r="X1" s="16"/>
+      <c r="Y1" s="16"/>
+      <c r="Z1" s="16"/>
     </row>
     <row r="2" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="20"/>
-      <c r="B2" s="20"/>
-      <c r="C2" s="20"/>
-      <c r="D2" s="20"/>
-      <c r="E2" s="20"/>
-      <c r="F2" s="20"/>
-      <c r="G2" s="20"/>
-      <c r="H2" s="20"/>
-      <c r="I2" s="20"/>
-      <c r="J2" s="20"/>
-      <c r="K2" s="20"/>
-      <c r="L2" s="20"/>
-      <c r="M2" s="20"/>
-      <c r="N2" s="20"/>
-      <c r="O2" s="20"/>
-      <c r="P2" s="20"/>
-      <c r="Q2" s="20"/>
-      <c r="R2" s="20"/>
-      <c r="S2" s="20"/>
-      <c r="T2" s="20"/>
-      <c r="U2" s="20"/>
-      <c r="V2" s="20"/>
-      <c r="W2" s="20"/>
-      <c r="X2" s="20"/>
-      <c r="Y2" s="20"/>
-      <c r="Z2" s="20"/>
+      <c r="A2" s="16"/>
+      <c r="B2" s="16"/>
+      <c r="C2" s="16"/>
+      <c r="D2" s="16"/>
+      <c r="E2" s="16"/>
+      <c r="F2" s="16"/>
+      <c r="G2" s="16"/>
+      <c r="H2" s="16"/>
+      <c r="I2" s="16"/>
+      <c r="J2" s="16"/>
+      <c r="K2" s="16"/>
+      <c r="L2" s="16"/>
+      <c r="M2" s="16"/>
+      <c r="N2" s="16"/>
+      <c r="O2" s="16"/>
+      <c r="P2" s="16"/>
+      <c r="Q2" s="16"/>
+      <c r="R2" s="16"/>
+      <c r="S2" s="16"/>
+      <c r="T2" s="16"/>
+      <c r="U2" s="16"/>
+      <c r="V2" s="16"/>
+      <c r="W2" s="16"/>
+      <c r="X2" s="16"/>
+      <c r="Y2" s="16"/>
+      <c r="Z2" s="16"/>
     </row>
     <row r="3" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="20"/>
-      <c r="B3" s="20"/>
-      <c r="C3" s="20"/>
-      <c r="D3" s="20"/>
-      <c r="E3" s="20"/>
-      <c r="F3" s="20"/>
-      <c r="G3" s="20"/>
-      <c r="H3" s="20"/>
-      <c r="I3" s="20"/>
-      <c r="J3" s="20"/>
-      <c r="K3" s="20"/>
-      <c r="L3" s="20"/>
-      <c r="M3" s="20"/>
-      <c r="N3" s="20"/>
-      <c r="O3" s="20"/>
-      <c r="P3" s="20"/>
-      <c r="Q3" s="20"/>
-      <c r="R3" s="20"/>
-      <c r="S3" s="20"/>
-      <c r="T3" s="20"/>
-      <c r="U3" s="20"/>
-      <c r="V3" s="20"/>
-      <c r="W3" s="20"/>
-      <c r="X3" s="20"/>
-      <c r="Y3" s="20"/>
-      <c r="Z3" s="20"/>
+      <c r="A3" s="16"/>
+      <c r="B3" s="16"/>
+      <c r="C3" s="16"/>
+      <c r="D3" s="16"/>
+      <c r="E3" s="16"/>
+      <c r="F3" s="16"/>
+      <c r="G3" s="16"/>
+      <c r="H3" s="16"/>
+      <c r="I3" s="16"/>
+      <c r="J3" s="16"/>
+      <c r="K3" s="16"/>
+      <c r="L3" s="16"/>
+      <c r="M3" s="16"/>
+      <c r="N3" s="16"/>
+      <c r="O3" s="16"/>
+      <c r="P3" s="16"/>
+      <c r="Q3" s="16"/>
+      <c r="R3" s="16"/>
+      <c r="S3" s="16"/>
+      <c r="T3" s="16"/>
+      <c r="U3" s="16"/>
+      <c r="V3" s="16"/>
+      <c r="W3" s="16"/>
+      <c r="X3" s="16"/>
+      <c r="Y3" s="16"/>
+      <c r="Z3" s="16"/>
     </row>
     <row r="4" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="20"/>
-      <c r="B4" s="20"/>
-      <c r="C4" s="20"/>
-      <c r="D4" s="20"/>
-      <c r="E4" s="20"/>
-      <c r="F4" s="20"/>
-      <c r="G4" s="20"/>
-      <c r="H4" s="20"/>
-      <c r="I4" s="20"/>
-      <c r="J4" s="20"/>
-      <c r="K4" s="20"/>
-      <c r="L4" s="20"/>
-      <c r="M4" s="20"/>
-      <c r="N4" s="20"/>
-      <c r="O4" s="20"/>
-      <c r="P4" s="20"/>
-      <c r="Q4" s="20"/>
-      <c r="R4" s="20"/>
-      <c r="S4" s="20"/>
-      <c r="T4" s="20"/>
-      <c r="U4" s="20"/>
-      <c r="V4" s="20"/>
-      <c r="W4" s="20"/>
-      <c r="X4" s="20"/>
-      <c r="Y4" s="20"/>
-      <c r="Z4" s="20"/>
+      <c r="A4" s="16"/>
+      <c r="B4" s="16"/>
+      <c r="C4" s="16"/>
+      <c r="D4" s="16"/>
+      <c r="E4" s="16"/>
+      <c r="F4" s="16"/>
+      <c r="G4" s="16"/>
+      <c r="H4" s="16"/>
+      <c r="I4" s="16"/>
+      <c r="J4" s="16"/>
+      <c r="K4" s="16"/>
+      <c r="L4" s="16"/>
+      <c r="M4" s="16"/>
+      <c r="N4" s="16"/>
+      <c r="O4" s="16"/>
+      <c r="P4" s="16"/>
+      <c r="Q4" s="16"/>
+      <c r="R4" s="16"/>
+      <c r="S4" s="16"/>
+      <c r="T4" s="16"/>
+      <c r="U4" s="16"/>
+      <c r="V4" s="16"/>
+      <c r="W4" s="16"/>
+      <c r="X4" s="16"/>
+      <c r="Y4" s="16"/>
+      <c r="Z4" s="16"/>
     </row>
     <row r="5" spans="1:26" ht="3" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="20"/>
-      <c r="B5" s="20"/>
-      <c r="C5" s="20"/>
-      <c r="D5" s="20"/>
-      <c r="E5" s="20"/>
-      <c r="F5" s="20"/>
-      <c r="G5" s="20"/>
-      <c r="H5" s="20"/>
-      <c r="I5" s="20"/>
-      <c r="J5" s="20"/>
-      <c r="K5" s="20"/>
-      <c r="L5" s="20"/>
-      <c r="M5" s="20"/>
-      <c r="N5" s="20"/>
-      <c r="O5" s="20"/>
-      <c r="P5" s="20"/>
-      <c r="Q5" s="20"/>
-      <c r="R5" s="20"/>
-      <c r="S5" s="20"/>
-      <c r="T5" s="20"/>
-      <c r="U5" s="20"/>
-      <c r="V5" s="20"/>
-      <c r="W5" s="20"/>
-      <c r="X5" s="20"/>
-      <c r="Y5" s="20"/>
-      <c r="Z5" s="20"/>
+      <c r="A5" s="16"/>
+      <c r="B5" s="16"/>
+      <c r="C5" s="16"/>
+      <c r="D5" s="16"/>
+      <c r="E5" s="16"/>
+      <c r="F5" s="16"/>
+      <c r="G5" s="16"/>
+      <c r="H5" s="16"/>
+      <c r="I5" s="16"/>
+      <c r="J5" s="16"/>
+      <c r="K5" s="16"/>
+      <c r="L5" s="16"/>
+      <c r="M5" s="16"/>
+      <c r="N5" s="16"/>
+      <c r="O5" s="16"/>
+      <c r="P5" s="16"/>
+      <c r="Q5" s="16"/>
+      <c r="R5" s="16"/>
+      <c r="S5" s="16"/>
+      <c r="T5" s="16"/>
+      <c r="U5" s="16"/>
+      <c r="V5" s="16"/>
+      <c r="W5" s="16"/>
+      <c r="X5" s="16"/>
+      <c r="Y5" s="16"/>
+      <c r="Z5" s="16"/>
     </row>
     <row r="6" spans="1:26" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="20"/>
-      <c r="B6" s="20"/>
-      <c r="C6" s="20"/>
-      <c r="D6" s="20"/>
-      <c r="E6" s="20"/>
-      <c r="F6" s="20"/>
-      <c r="G6" s="20"/>
-      <c r="H6" s="20"/>
-      <c r="I6" s="20"/>
-      <c r="J6" s="20"/>
-      <c r="K6" s="20"/>
-      <c r="L6" s="20"/>
-      <c r="M6" s="20"/>
-      <c r="N6" s="20"/>
-      <c r="O6" s="20"/>
-      <c r="P6" s="20"/>
-      <c r="Q6" s="20"/>
-      <c r="R6" s="20"/>
-      <c r="S6" s="20"/>
-      <c r="T6" s="20"/>
-      <c r="U6" s="20"/>
-      <c r="V6" s="20"/>
-      <c r="W6" s="20"/>
-      <c r="X6" s="20"/>
-      <c r="Y6" s="20"/>
-      <c r="Z6" s="20"/>
+      <c r="A6" s="16"/>
+      <c r="B6" s="16"/>
+      <c r="C6" s="16"/>
+      <c r="D6" s="16"/>
+      <c r="E6" s="16"/>
+      <c r="F6" s="16"/>
+      <c r="G6" s="16"/>
+      <c r="H6" s="16"/>
+      <c r="I6" s="16"/>
+      <c r="J6" s="16"/>
+      <c r="K6" s="16"/>
+      <c r="L6" s="16"/>
+      <c r="M6" s="16"/>
+      <c r="N6" s="16"/>
+      <c r="O6" s="16"/>
+      <c r="P6" s="16"/>
+      <c r="Q6" s="16"/>
+      <c r="R6" s="16"/>
+      <c r="S6" s="16"/>
+      <c r="T6" s="16"/>
+      <c r="U6" s="16"/>
+      <c r="V6" s="16"/>
+      <c r="W6" s="16"/>
+      <c r="X6" s="16"/>
+      <c r="Y6" s="16"/>
+      <c r="Z6" s="16"/>
     </row>
     <row r="7" spans="1:26" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="20"/>
-      <c r="B7" s="20"/>
-      <c r="C7" s="20"/>
-      <c r="D7" s="20"/>
-      <c r="E7" s="20"/>
-      <c r="F7" s="20"/>
-      <c r="G7" s="20"/>
-      <c r="H7" s="20"/>
-      <c r="I7" s="20"/>
-      <c r="J7" s="20"/>
-      <c r="K7" s="20"/>
-      <c r="L7" s="20"/>
-      <c r="M7" s="20"/>
-      <c r="N7" s="20"/>
-      <c r="O7" s="20"/>
-      <c r="P7" s="20"/>
-      <c r="Q7" s="20"/>
-      <c r="R7" s="20"/>
-      <c r="S7" s="20"/>
-      <c r="T7" s="20"/>
-      <c r="U7" s="20"/>
-      <c r="V7" s="20"/>
-      <c r="W7" s="20"/>
-      <c r="X7" s="20"/>
-      <c r="Y7" s="20"/>
-      <c r="Z7" s="20"/>
+      <c r="A7" s="16"/>
+      <c r="B7" s="16"/>
+      <c r="C7" s="16"/>
+      <c r="D7" s="16"/>
+      <c r="E7" s="16"/>
+      <c r="F7" s="16"/>
+      <c r="G7" s="16"/>
+      <c r="H7" s="16"/>
+      <c r="I7" s="16"/>
+      <c r="J7" s="16"/>
+      <c r="K7" s="16"/>
+      <c r="L7" s="16"/>
+      <c r="M7" s="16"/>
+      <c r="N7" s="16"/>
+      <c r="O7" s="16"/>
+      <c r="P7" s="16"/>
+      <c r="Q7" s="16"/>
+      <c r="R7" s="16"/>
+      <c r="S7" s="16"/>
+      <c r="T7" s="16"/>
+      <c r="U7" s="16"/>
+      <c r="V7" s="16"/>
+      <c r="W7" s="16"/>
+      <c r="X7" s="16"/>
+      <c r="Y7" s="16"/>
+      <c r="Z7" s="16"/>
     </row>
     <row r="8" spans="1:26" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="20"/>
-      <c r="B8" s="20"/>
-      <c r="C8" s="20"/>
-      <c r="D8" s="20"/>
-      <c r="E8" s="20"/>
-      <c r="F8" s="20"/>
-      <c r="G8" s="20"/>
-      <c r="H8" s="20"/>
-      <c r="I8" s="20"/>
-      <c r="J8" s="20"/>
-      <c r="K8" s="20"/>
-      <c r="L8" s="20"/>
-      <c r="M8" s="20"/>
-      <c r="N8" s="20"/>
-      <c r="O8" s="20"/>
-      <c r="P8" s="20"/>
-      <c r="Q8" s="20"/>
-      <c r="R8" s="20"/>
-      <c r="S8" s="20"/>
-      <c r="T8" s="20"/>
-      <c r="U8" s="20"/>
-      <c r="V8" s="20"/>
-      <c r="W8" s="20"/>
-      <c r="X8" s="20"/>
-      <c r="Y8" s="20"/>
-      <c r="Z8" s="20"/>
+      <c r="A8" s="16"/>
+      <c r="B8" s="16"/>
+      <c r="C8" s="16"/>
+      <c r="D8" s="16"/>
+      <c r="E8" s="16"/>
+      <c r="F8" s="16"/>
+      <c r="G8" s="16"/>
+      <c r="H8" s="16"/>
+      <c r="I8" s="16"/>
+      <c r="J8" s="16"/>
+      <c r="K8" s="16"/>
+      <c r="L8" s="16"/>
+      <c r="M8" s="16"/>
+      <c r="N8" s="16"/>
+      <c r="O8" s="16"/>
+      <c r="P8" s="16"/>
+      <c r="Q8" s="16"/>
+      <c r="R8" s="16"/>
+      <c r="S8" s="16"/>
+      <c r="T8" s="16"/>
+      <c r="U8" s="16"/>
+      <c r="V8" s="16"/>
+      <c r="W8" s="16"/>
+      <c r="X8" s="16"/>
+      <c r="Y8" s="16"/>
+      <c r="Z8" s="16"/>
     </row>
     <row r="9" spans="1:26" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="20"/>
-      <c r="B9" s="20"/>
-      <c r="C9" s="20"/>
-      <c r="D9" s="20"/>
-      <c r="E9" s="20"/>
-      <c r="F9" s="20"/>
-      <c r="G9" s="20"/>
-      <c r="H9" s="20"/>
-      <c r="I9" s="20"/>
-      <c r="J9" s="20"/>
-      <c r="K9" s="20"/>
-      <c r="L9" s="20"/>
-      <c r="M9" s="20"/>
-      <c r="N9" s="20"/>
-      <c r="O9" s="20"/>
-      <c r="P9" s="20"/>
-      <c r="Q9" s="20"/>
-      <c r="R9" s="20"/>
-      <c r="S9" s="20"/>
-      <c r="T9" s="20"/>
-      <c r="U9" s="20"/>
-      <c r="V9" s="20"/>
-      <c r="W9" s="20"/>
-      <c r="X9" s="20"/>
-      <c r="Y9" s="20"/>
-      <c r="Z9" s="20"/>
+      <c r="A9" s="16"/>
+      <c r="B9" s="16"/>
+      <c r="C9" s="16"/>
+      <c r="D9" s="16"/>
+      <c r="E9" s="16"/>
+      <c r="F9" s="16"/>
+      <c r="G9" s="16"/>
+      <c r="H9" s="16"/>
+      <c r="I9" s="16"/>
+      <c r="J9" s="16"/>
+      <c r="K9" s="16"/>
+      <c r="L9" s="16"/>
+      <c r="M9" s="16"/>
+      <c r="N9" s="16"/>
+      <c r="O9" s="16"/>
+      <c r="P9" s="16"/>
+      <c r="Q9" s="16"/>
+      <c r="R9" s="16"/>
+      <c r="S9" s="16"/>
+      <c r="T9" s="16"/>
+      <c r="U9" s="16"/>
+      <c r="V9" s="16"/>
+      <c r="W9" s="16"/>
+      <c r="X9" s="16"/>
+      <c r="Y9" s="16"/>
+      <c r="Z9" s="16"/>
     </row>
     <row r="10" spans="1:26" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="20"/>
-      <c r="B10" s="20"/>
-      <c r="C10" s="20"/>
-      <c r="D10" s="20"/>
-      <c r="E10" s="20"/>
-      <c r="F10" s="20"/>
-      <c r="G10" s="20"/>
-      <c r="H10" s="20"/>
-      <c r="I10" s="20"/>
-      <c r="J10" s="20"/>
-      <c r="K10" s="20"/>
-      <c r="L10" s="20"/>
-      <c r="M10" s="20"/>
-      <c r="N10" s="20"/>
-      <c r="O10" s="20"/>
-      <c r="P10" s="20"/>
-      <c r="Q10" s="20"/>
-      <c r="R10" s="20"/>
-      <c r="S10" s="20"/>
-      <c r="T10" s="20"/>
-      <c r="U10" s="20"/>
-      <c r="V10" s="20"/>
-      <c r="W10" s="20"/>
-      <c r="X10" s="20"/>
-      <c r="Y10" s="20"/>
-      <c r="Z10" s="20"/>
+      <c r="A10" s="16"/>
+      <c r="B10" s="16"/>
+      <c r="C10" s="16"/>
+      <c r="D10" s="16"/>
+      <c r="E10" s="16"/>
+      <c r="F10" s="16"/>
+      <c r="G10" s="16"/>
+      <c r="H10" s="16"/>
+      <c r="I10" s="16"/>
+      <c r="J10" s="16"/>
+      <c r="K10" s="16"/>
+      <c r="L10" s="16"/>
+      <c r="M10" s="16"/>
+      <c r="N10" s="16"/>
+      <c r="O10" s="16"/>
+      <c r="P10" s="16"/>
+      <c r="Q10" s="16"/>
+      <c r="R10" s="16"/>
+      <c r="S10" s="16"/>
+      <c r="T10" s="16"/>
+      <c r="U10" s="16"/>
+      <c r="V10" s="16"/>
+      <c r="W10" s="16"/>
+      <c r="X10" s="16"/>
+      <c r="Y10" s="16"/>
+      <c r="Z10" s="16"/>
     </row>
     <row r="11" spans="1:26" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="20"/>
-      <c r="B11" s="20"/>
-      <c r="C11" s="20"/>
-      <c r="D11" s="20"/>
-      <c r="E11" s="20"/>
-      <c r="F11" s="20"/>
-      <c r="G11" s="20"/>
-      <c r="H11" s="20"/>
-      <c r="I11" s="20"/>
-      <c r="J11" s="20"/>
-      <c r="K11" s="20"/>
-      <c r="L11" s="20"/>
-      <c r="M11" s="20"/>
-      <c r="N11" s="20"/>
-      <c r="O11" s="20"/>
-      <c r="P11" s="20"/>
-      <c r="Q11" s="20"/>
-      <c r="R11" s="20"/>
-      <c r="S11" s="20"/>
-      <c r="T11" s="20"/>
-      <c r="U11" s="20"/>
-      <c r="V11" s="20"/>
-      <c r="W11" s="20"/>
-      <c r="X11" s="20"/>
-      <c r="Y11" s="20"/>
-      <c r="Z11" s="20"/>
+      <c r="A11" s="16"/>
+      <c r="B11" s="16"/>
+      <c r="C11" s="16"/>
+      <c r="D11" s="16"/>
+      <c r="E11" s="16"/>
+      <c r="F11" s="16"/>
+      <c r="G11" s="16"/>
+      <c r="H11" s="16"/>
+      <c r="I11" s="16"/>
+      <c r="J11" s="16"/>
+      <c r="K11" s="16"/>
+      <c r="L11" s="16"/>
+      <c r="M11" s="16"/>
+      <c r="N11" s="16"/>
+      <c r="O11" s="16"/>
+      <c r="P11" s="16"/>
+      <c r="Q11" s="16"/>
+      <c r="R11" s="16"/>
+      <c r="S11" s="16"/>
+      <c r="T11" s="16"/>
+      <c r="U11" s="16"/>
+      <c r="V11" s="16"/>
+      <c r="W11" s="16"/>
+      <c r="X11" s="16"/>
+      <c r="Y11" s="16"/>
+      <c r="Z11" s="16"/>
     </row>
     <row r="14" spans="1:26" x14ac:dyDescent="0.25">
       <c r="G14" s="17" t="s">
@@ -1229,20 +2104,20 @@
       </c>
       <c r="H14" s="18"/>
       <c r="I14" s="19"/>
-      <c r="K14" s="9" t="s">
+      <c r="K14" s="20" t="s">
         <v>26</v>
       </c>
-      <c r="L14" s="10"/>
-      <c r="M14" s="10"/>
-      <c r="N14" s="10"/>
-      <c r="O14" s="10"/>
-      <c r="P14" s="10"/>
-      <c r="Q14" s="10"/>
-      <c r="R14" s="10"/>
-      <c r="S14" s="10"/>
-      <c r="T14" s="10"/>
-      <c r="U14" s="10"/>
-      <c r="V14" s="11"/>
+      <c r="L14" s="21"/>
+      <c r="M14" s="21"/>
+      <c r="N14" s="21"/>
+      <c r="O14" s="21"/>
+      <c r="P14" s="21"/>
+      <c r="Q14" s="21"/>
+      <c r="R14" s="21"/>
+      <c r="S14" s="21"/>
+      <c r="T14" s="21"/>
+      <c r="U14" s="21"/>
+      <c r="V14" s="22"/>
     </row>
     <row r="15" spans="1:26" x14ac:dyDescent="0.25">
       <c r="G15" s="17" t="s">
@@ -1250,20 +2125,20 @@
       </c>
       <c r="H15" s="18"/>
       <c r="I15" s="19"/>
-      <c r="K15" s="21" t="s">
+      <c r="K15" s="23" t="s">
         <v>27</v>
       </c>
-      <c r="L15" s="10"/>
-      <c r="M15" s="10"/>
-      <c r="N15" s="10"/>
-      <c r="O15" s="10"/>
-      <c r="P15" s="10"/>
-      <c r="Q15" s="10"/>
-      <c r="R15" s="10"/>
-      <c r="S15" s="10"/>
-      <c r="T15" s="10"/>
-      <c r="U15" s="10"/>
-      <c r="V15" s="11"/>
+      <c r="L15" s="21"/>
+      <c r="M15" s="21"/>
+      <c r="N15" s="21"/>
+      <c r="O15" s="21"/>
+      <c r="P15" s="21"/>
+      <c r="Q15" s="21"/>
+      <c r="R15" s="21"/>
+      <c r="S15" s="21"/>
+      <c r="T15" s="21"/>
+      <c r="U15" s="21"/>
+      <c r="V15" s="22"/>
     </row>
     <row r="16" spans="1:26" x14ac:dyDescent="0.25">
       <c r="G16" s="17" t="s">
@@ -1271,20 +2146,20 @@
       </c>
       <c r="H16" s="18"/>
       <c r="I16" s="19"/>
-      <c r="K16" s="12" t="s">
+      <c r="K16" s="24" t="s">
         <v>7</v>
       </c>
-      <c r="L16" s="13"/>
-      <c r="M16" s="13"/>
-      <c r="N16" s="13"/>
-      <c r="O16" s="13"/>
-      <c r="P16" s="13"/>
-      <c r="Q16" s="13"/>
-      <c r="R16" s="13"/>
-      <c r="S16" s="13"/>
-      <c r="T16" s="13"/>
-      <c r="U16" s="13"/>
-      <c r="V16" s="14"/>
+      <c r="L16" s="25"/>
+      <c r="M16" s="25"/>
+      <c r="N16" s="25"/>
+      <c r="O16" s="25"/>
+      <c r="P16" s="25"/>
+      <c r="Q16" s="25"/>
+      <c r="R16" s="25"/>
+      <c r="S16" s="25"/>
+      <c r="T16" s="25"/>
+      <c r="U16" s="25"/>
+      <c r="V16" s="26"/>
     </row>
     <row r="19" spans="7:22" x14ac:dyDescent="0.25">
       <c r="G19" s="17" t="s">
@@ -1292,20 +2167,20 @@
       </c>
       <c r="H19" s="18"/>
       <c r="I19" s="19"/>
-      <c r="K19" s="9" t="s">
+      <c r="K19" s="20" t="s">
         <v>8</v>
       </c>
-      <c r="L19" s="10"/>
-      <c r="M19" s="10"/>
-      <c r="N19" s="10"/>
-      <c r="O19" s="10"/>
-      <c r="P19" s="10"/>
-      <c r="Q19" s="10"/>
-      <c r="R19" s="10"/>
-      <c r="S19" s="10"/>
-      <c r="T19" s="10"/>
-      <c r="U19" s="10"/>
-      <c r="V19" s="11"/>
+      <c r="L19" s="21"/>
+      <c r="M19" s="21"/>
+      <c r="N19" s="21"/>
+      <c r="O19" s="21"/>
+      <c r="P19" s="21"/>
+      <c r="Q19" s="21"/>
+      <c r="R19" s="21"/>
+      <c r="S19" s="21"/>
+      <c r="T19" s="21"/>
+      <c r="U19" s="21"/>
+      <c r="V19" s="22"/>
     </row>
     <row r="20" spans="7:22" x14ac:dyDescent="0.25">
       <c r="G20" s="17" t="s">
@@ -1313,20 +2188,20 @@
       </c>
       <c r="H20" s="18"/>
       <c r="I20" s="19"/>
-      <c r="K20" s="9" t="s">
+      <c r="K20" s="20" t="s">
         <v>9</v>
       </c>
-      <c r="L20" s="10"/>
-      <c r="M20" s="10"/>
-      <c r="N20" s="10"/>
-      <c r="O20" s="10"/>
-      <c r="P20" s="10"/>
-      <c r="Q20" s="10"/>
-      <c r="R20" s="10"/>
-      <c r="S20" s="10"/>
-      <c r="T20" s="10"/>
-      <c r="U20" s="10"/>
-      <c r="V20" s="11"/>
+      <c r="L20" s="21"/>
+      <c r="M20" s="21"/>
+      <c r="N20" s="21"/>
+      <c r="O20" s="21"/>
+      <c r="P20" s="21"/>
+      <c r="Q20" s="21"/>
+      <c r="R20" s="21"/>
+      <c r="S20" s="21"/>
+      <c r="T20" s="21"/>
+      <c r="U20" s="21"/>
+      <c r="V20" s="22"/>
     </row>
     <row r="21" spans="7:22" x14ac:dyDescent="0.25">
       <c r="G21" s="17" t="s">
@@ -1334,20 +2209,20 @@
       </c>
       <c r="H21" s="18"/>
       <c r="I21" s="19"/>
-      <c r="K21" s="12" t="s">
+      <c r="K21" s="24" t="s">
         <v>10</v>
       </c>
-      <c r="L21" s="13"/>
-      <c r="M21" s="13"/>
-      <c r="N21" s="13"/>
-      <c r="O21" s="13"/>
-      <c r="P21" s="13"/>
-      <c r="Q21" s="13"/>
-      <c r="R21" s="13"/>
-      <c r="S21" s="13"/>
-      <c r="T21" s="13"/>
-      <c r="U21" s="13"/>
-      <c r="V21" s="14"/>
+      <c r="L21" s="25"/>
+      <c r="M21" s="25"/>
+      <c r="N21" s="25"/>
+      <c r="O21" s="25"/>
+      <c r="P21" s="25"/>
+      <c r="Q21" s="25"/>
+      <c r="R21" s="25"/>
+      <c r="S21" s="25"/>
+      <c r="T21" s="25"/>
+      <c r="U21" s="25"/>
+      <c r="V21" s="26"/>
     </row>
     <row r="24" spans="7:22" x14ac:dyDescent="0.25">
       <c r="G24" s="17" t="s">
@@ -1355,30 +2230,23 @@
       </c>
       <c r="H24" s="18"/>
       <c r="I24" s="19"/>
-      <c r="K24" s="15">
+      <c r="K24" s="27">
         <v>45439</v>
       </c>
-      <c r="L24" s="16"/>
-      <c r="M24" s="16"/>
-      <c r="N24" s="16"/>
-      <c r="O24" s="16"/>
-      <c r="P24" s="16"/>
-      <c r="Q24" s="16"/>
-      <c r="R24" s="16"/>
-      <c r="S24" s="16"/>
-      <c r="T24" s="16"/>
-      <c r="U24" s="16"/>
-      <c r="V24" s="16"/>
+      <c r="L24" s="28"/>
+      <c r="M24" s="28"/>
+      <c r="N24" s="28"/>
+      <c r="O24" s="28"/>
+      <c r="P24" s="28"/>
+      <c r="Q24" s="28"/>
+      <c r="R24" s="28"/>
+      <c r="S24" s="28"/>
+      <c r="T24" s="28"/>
+      <c r="U24" s="28"/>
+      <c r="V24" s="28"/>
     </row>
   </sheetData>
   <mergeCells count="15">
-    <mergeCell ref="A1:Z11"/>
-    <mergeCell ref="G14:I14"/>
-    <mergeCell ref="K14:V14"/>
-    <mergeCell ref="G15:I15"/>
-    <mergeCell ref="G16:I16"/>
-    <mergeCell ref="K15:V15"/>
-    <mergeCell ref="K16:V16"/>
     <mergeCell ref="K19:V19"/>
     <mergeCell ref="K20:V20"/>
     <mergeCell ref="K21:V21"/>
@@ -1387,6 +2255,13 @@
     <mergeCell ref="G20:I20"/>
     <mergeCell ref="G21:I21"/>
     <mergeCell ref="G24:I24"/>
+    <mergeCell ref="A1:Z11"/>
+    <mergeCell ref="G14:I14"/>
+    <mergeCell ref="K14:V14"/>
+    <mergeCell ref="G15:I15"/>
+    <mergeCell ref="G16:I16"/>
+    <mergeCell ref="K15:V15"/>
+    <mergeCell ref="K16:V16"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="K15" r:id="rId1" xr:uid="{B39E7FA7-0077-4592-BE7E-C6FE950055E9}"/>
@@ -1400,7 +2275,7 @@
   <dimension ref="A1:I21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C26" sqref="C26"/>
+      <selection activeCell="C23" sqref="C23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1459,7 +2334,7 @@
       <c r="H2" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="I2" s="25" t="s">
+      <c r="I2" s="9" t="s">
         <v>50</v>
       </c>
     </row>
@@ -1486,7 +2361,7 @@
       <c r="H3" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="I3" s="25" t="s">
+      <c r="I3" s="9" t="s">
         <v>50</v>
       </c>
     </row>
@@ -1513,7 +2388,7 @@
       <c r="H4" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="I4" s="25" t="s">
+      <c r="I4" s="9" t="s">
         <v>50</v>
       </c>
     </row>
@@ -1540,7 +2415,7 @@
       <c r="H5" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="I5" s="25" t="s">
+      <c r="I5" s="9" t="s">
         <v>50</v>
       </c>
     </row>
@@ -1567,7 +2442,7 @@
       <c r="H6" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="I6" s="25" t="s">
+      <c r="I6" s="9" t="s">
         <v>50</v>
       </c>
     </row>
@@ -1596,36 +2471,36 @@
       <c r="H7" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="I7" s="25" t="s">
+      <c r="I7" s="9" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A8" s="27">
+      <c r="A8" s="11">
         <v>7</v>
       </c>
-      <c r="B8" s="27" t="s">
+      <c r="B8" s="11" t="s">
         <v>42</v>
       </c>
-      <c r="C8" s="27">
+      <c r="C8" s="11">
         <v>6</v>
       </c>
-      <c r="D8" s="27" t="s">
+      <c r="D8" s="11" t="s">
         <v>48</v>
       </c>
-      <c r="E8" s="27" t="s">
+      <c r="E8" s="11" t="s">
         <v>49</v>
       </c>
-      <c r="F8" s="27" t="s">
+      <c r="F8" s="11" t="s">
         <v>34</v>
       </c>
-      <c r="G8" s="27" t="s">
+      <c r="G8" s="11" t="s">
         <v>59</v>
       </c>
-      <c r="H8" s="27" t="s">
+      <c r="H8" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="I8" s="28" t="s">
+      <c r="I8" s="12" t="s">
         <v>50</v>
       </c>
     </row>
@@ -1646,7 +2521,7 @@
       <c r="H9" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="I9" s="26" t="s">
+      <c r="I9" s="10" t="s">
         <v>51</v>
       </c>
     </row>
@@ -1673,7 +2548,7 @@
       <c r="H10" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="I10" s="26" t="s">
+      <c r="I10" s="10" t="s">
         <v>51</v>
       </c>
     </row>
@@ -1700,7 +2575,7 @@
       <c r="H11" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="I11" s="26" t="s">
+      <c r="I11" s="10" t="s">
         <v>51</v>
       </c>
     </row>
@@ -1727,7 +2602,7 @@
       <c r="H12" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="I12" s="26" t="s">
+      <c r="I12" s="10" t="s">
         <v>51</v>
       </c>
     </row>
@@ -1754,7 +2629,7 @@
       <c r="H13" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="I13" s="26" t="s">
+      <c r="I13" s="10" t="s">
         <v>51</v>
       </c>
     </row>
@@ -1783,36 +2658,36 @@
       <c r="H14" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="I14" s="26" t="s">
+      <c r="I14" s="10" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A15" s="27">
+      <c r="A15" s="11">
         <v>14</v>
       </c>
-      <c r="B15" s="27" t="s">
+      <c r="B15" s="11" t="s">
         <v>47</v>
       </c>
-      <c r="C15" s="27">
+      <c r="C15" s="11">
         <v>13</v>
       </c>
-      <c r="D15" s="27" t="s">
+      <c r="D15" s="11" t="s">
         <v>48</v>
       </c>
-      <c r="E15" s="27" t="s">
+      <c r="E15" s="11" t="s">
         <v>49</v>
       </c>
-      <c r="F15" s="27" t="s">
+      <c r="F15" s="11" t="s">
         <v>34</v>
       </c>
-      <c r="G15" s="27" t="s">
+      <c r="G15" s="11" t="s">
         <v>60</v>
       </c>
-      <c r="H15" s="27" t="s">
+      <c r="H15" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="I15" s="29" t="s">
+      <c r="I15" s="13" t="s">
         <v>51</v>
       </c>
     </row>
@@ -1823,23 +2698,15 @@
       <c r="B16" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="C16" s="1">
-        <v>14</v>
-      </c>
-      <c r="D16" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="E16" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="F16" s="1" t="s">
-        <v>34</v>
-      </c>
+      <c r="C16" s="1"/>
+      <c r="D16" s="1"/>
+      <c r="E16" s="1"/>
+      <c r="F16" s="1"/>
       <c r="G16" s="8"/>
       <c r="H16" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="I16" s="30" t="s">
+      <c r="I16" s="14" t="s">
         <v>61</v>
       </c>
     </row>
@@ -1850,23 +2717,15 @@
       <c r="B17" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="C17" s="1">
-        <v>15</v>
-      </c>
-      <c r="D17" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="E17" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="F17" s="1" t="s">
-        <v>34</v>
-      </c>
+      <c r="C17" s="1"/>
+      <c r="D17" s="1"/>
+      <c r="E17" s="1"/>
+      <c r="F17" s="1"/>
       <c r="G17" s="8"/>
       <c r="H17" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="I17" s="30" t="s">
+      <c r="I17" s="14" t="s">
         <v>61</v>
       </c>
     </row>
@@ -1877,23 +2736,15 @@
       <c r="B18" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="C18" s="1">
-        <v>16</v>
-      </c>
-      <c r="D18" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="E18" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="F18" s="1" t="s">
-        <v>34</v>
-      </c>
+      <c r="C18" s="1"/>
+      <c r="D18" s="1"/>
+      <c r="E18" s="1"/>
+      <c r="F18" s="1"/>
       <c r="G18" s="8"/>
       <c r="H18" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="I18" s="30" t="s">
+      <c r="I18" s="14" t="s">
         <v>61</v>
       </c>
     </row>
@@ -1904,23 +2755,15 @@
       <c r="B19" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="C19" s="1">
-        <v>17</v>
-      </c>
-      <c r="D19" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="E19" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="F19" s="1" t="s">
-        <v>34</v>
-      </c>
+      <c r="C19" s="1"/>
+      <c r="D19" s="1"/>
+      <c r="E19" s="1"/>
+      <c r="F19" s="1"/>
       <c r="G19" s="8"/>
       <c r="H19" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="I19" s="30" t="s">
+      <c r="I19" s="14" t="s">
         <v>61</v>
       </c>
     </row>
@@ -1931,23 +2774,15 @@
       <c r="B20" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="C20" s="1">
-        <v>18</v>
-      </c>
-      <c r="D20" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="E20" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="F20" s="1" t="s">
-        <v>34</v>
-      </c>
+      <c r="C20" s="1"/>
+      <c r="D20" s="1"/>
+      <c r="E20" s="1"/>
+      <c r="F20" s="1"/>
       <c r="G20" s="8"/>
       <c r="H20" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="I20" s="30" t="s">
+      <c r="I20" s="14" t="s">
         <v>61</v>
       </c>
     </row>
@@ -1956,25 +2791,17 @@
         <v>20</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="C21" s="1">
-        <v>19</v>
-      </c>
-      <c r="D21" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="E21" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="F21" s="1" t="s">
-        <v>34</v>
-      </c>
+        <v>158</v>
+      </c>
+      <c r="C21" s="1"/>
+      <c r="D21" s="1"/>
+      <c r="E21" s="1"/>
+      <c r="F21" s="1"/>
       <c r="G21" s="8"/>
       <c r="H21" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="I21" s="30" t="s">
+      <c r="I21" s="14" t="s">
         <v>61</v>
       </c>
     </row>
@@ -1990,10 +2817,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E2C1E1C6-748F-4782-83CA-6948B67C52D3}">
-  <dimension ref="A1:H83"/>
+  <dimension ref="A1:H98"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+    <sheetView topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="H24" sqref="H24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2035,32 +2862,32 @@
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2" s="22" t="s">
+      <c r="A2" s="29" t="s">
         <v>50</v>
       </c>
-      <c r="B2" s="23"/>
-      <c r="C2" s="23"/>
-      <c r="D2" s="23"/>
-      <c r="E2" s="23"/>
-      <c r="F2" s="23"/>
-      <c r="G2" s="23"/>
-      <c r="H2" s="24"/>
+      <c r="B2" s="30"/>
+      <c r="C2" s="30"/>
+      <c r="D2" s="30"/>
+      <c r="E2" s="30"/>
+      <c r="F2" s="30"/>
+      <c r="G2" s="30"/>
+      <c r="H2" s="31"/>
     </row>
     <row r="3" spans="1:8" ht="45" x14ac:dyDescent="0.25">
-      <c r="A3" s="31">
+      <c r="A3" s="15">
         <v>1</v>
       </c>
       <c r="B3" s="4" t="s">
+        <v>120</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="D3" s="4" t="s">
         <v>71</v>
       </c>
-      <c r="C3" s="4" t="s">
+      <c r="E3" s="4" t="s">
         <v>72</v>
-      </c>
-      <c r="D3" s="4" t="s">
-        <v>73</v>
-      </c>
-      <c r="E3" s="4" t="s">
-        <v>74</v>
       </c>
       <c r="F3" s="6" t="s">
         <v>20</v>
@@ -2075,16 +2902,16 @@
         <v>2</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>75</v>
+        <v>121</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>82</v>
+        <v>74</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="F4" s="6" t="s">
         <v>20</v>
@@ -2097,16 +2924,16 @@
         <v>3</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>76</v>
+        <v>122</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>81</v>
+        <v>73</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="F5" s="6" t="s">
         <v>20</v>
@@ -2119,16 +2946,16 @@
         <v>4</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>77</v>
+        <v>123</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>83</v>
+        <v>75</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="E6" s="4" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="F6" s="6" t="s">
         <v>20</v>
@@ -2141,16 +2968,16 @@
         <v>5</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>78</v>
+        <v>124</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>84</v>
+        <v>76</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="E7" s="4" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="F7" s="6" t="s">
         <v>20</v>
@@ -2163,16 +2990,16 @@
         <v>6</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>79</v>
+        <v>125</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>85</v>
+        <v>77</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="E8" s="4" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="F8" s="6" t="s">
         <v>20</v>
@@ -2185,400 +3012,790 @@
         <v>7</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>80</v>
+        <v>192</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>86</v>
+        <v>193</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>87</v>
+        <v>194</v>
       </c>
       <c r="E9" s="4" t="s">
-        <v>88</v>
-      </c>
-      <c r="F9" s="6" t="s">
+        <v>199</v>
+      </c>
+      <c r="F9" s="37" t="s">
+        <v>195</v>
+      </c>
+      <c r="G9" s="5" t="s">
+        <v>200</v>
+      </c>
+      <c r="H9" s="3" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" ht="120" x14ac:dyDescent="0.25">
+      <c r="A10" s="3">
+        <v>8</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>109</v>
+      </c>
+      <c r="C10" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="D10" s="4" t="s">
+        <v>110</v>
+      </c>
+      <c r="E10" s="4" t="s">
+        <v>111</v>
+      </c>
+      <c r="F10" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="G9" s="5"/>
-      <c r="H9" s="3"/>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A10" s="22" t="s">
-        <v>51</v>
-      </c>
-      <c r="B10" s="23"/>
-      <c r="C10" s="23"/>
-      <c r="D10" s="23"/>
-      <c r="E10" s="23"/>
-      <c r="F10" s="23"/>
-      <c r="G10" s="23"/>
-      <c r="H10" s="24"/>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A11" s="3"/>
-      <c r="B11" s="3"/>
-      <c r="C11" s="3"/>
-      <c r="D11" s="3"/>
-      <c r="E11" s="3"/>
-      <c r="F11" s="5"/>
+      <c r="G10" s="5"/>
+      <c r="H10" s="3"/>
+    </row>
+    <row r="11" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="A11" s="3">
+        <v>9</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>126</v>
+      </c>
+      <c r="C11" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="D11" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="E11" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="F11" s="6" t="s">
+        <v>20</v>
+      </c>
       <c r="G11" s="5"/>
       <c r="H11" s="3"/>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A12" s="3"/>
-      <c r="B12" s="3"/>
-      <c r="C12" s="3"/>
-      <c r="D12" s="3"/>
-      <c r="E12" s="3"/>
-      <c r="F12" s="5"/>
+    <row r="12" spans="1:8" ht="135" x14ac:dyDescent="0.25">
+      <c r="A12" s="3">
+        <v>10</v>
+      </c>
+      <c r="B12" s="4" t="s">
+        <v>126</v>
+      </c>
+      <c r="C12" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="D12" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="E12" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="F12" s="6" t="s">
+        <v>20</v>
+      </c>
       <c r="G12" s="5"/>
       <c r="H12" s="3"/>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A13" s="3"/>
-      <c r="B13" s="3"/>
-      <c r="C13" s="3"/>
-      <c r="D13" s="3"/>
-      <c r="E13" s="3"/>
-      <c r="F13" s="5"/>
-      <c r="G13" s="5"/>
-      <c r="H13" s="3"/>
+    <row r="13" spans="1:8" ht="120" x14ac:dyDescent="0.25">
+      <c r="A13" s="32">
+        <v>11</v>
+      </c>
+      <c r="B13" s="33" t="s">
+        <v>127</v>
+      </c>
+      <c r="C13" s="33" t="s">
+        <v>78</v>
+      </c>
+      <c r="D13" s="33" t="s">
+        <v>79</v>
+      </c>
+      <c r="E13" s="33" t="s">
+        <v>80</v>
+      </c>
+      <c r="F13" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="G13" s="34"/>
+      <c r="H13" s="32"/>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A14" s="22" t="s">
-        <v>68</v>
-      </c>
-      <c r="B14" s="23"/>
-      <c r="C14" s="23"/>
-      <c r="D14" s="23"/>
-      <c r="E14" s="23"/>
-      <c r="F14" s="23"/>
-      <c r="G14" s="23"/>
-      <c r="H14" s="24"/>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A15" s="3"/>
-      <c r="B15" s="3"/>
-      <c r="C15" s="3"/>
-      <c r="D15" s="3"/>
-      <c r="E15" s="3"/>
-      <c r="F15" s="5"/>
-      <c r="G15" s="5"/>
-      <c r="H15" s="3"/>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A16" s="3"/>
-      <c r="B16" s="3"/>
-      <c r="C16" s="3"/>
-      <c r="D16" s="3"/>
-      <c r="E16" s="3"/>
-      <c r="F16" s="5"/>
-      <c r="G16" s="5"/>
-      <c r="H16" s="3"/>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A17" s="3"/>
-      <c r="B17" s="3"/>
-      <c r="C17" s="3"/>
-      <c r="D17" s="3"/>
-      <c r="E17" s="3"/>
-      <c r="F17" s="5"/>
-      <c r="G17" s="5"/>
-      <c r="H17" s="3"/>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A18" s="22" t="s">
-        <v>61</v>
-      </c>
-      <c r="B18" s="23"/>
-      <c r="C18" s="23"/>
-      <c r="D18" s="23"/>
-      <c r="E18" s="23"/>
-      <c r="F18" s="23"/>
-      <c r="G18" s="23"/>
-      <c r="H18" s="24"/>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A19" s="3"/>
-      <c r="B19" s="3"/>
-      <c r="C19" s="3"/>
-      <c r="D19" s="3"/>
-      <c r="E19" s="3"/>
-      <c r="F19" s="5"/>
-      <c r="G19" s="5"/>
-      <c r="H19" s="3"/>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A20" s="3"/>
-      <c r="B20" s="3"/>
-      <c r="C20" s="3"/>
-      <c r="D20" s="3"/>
-      <c r="E20" s="3"/>
-      <c r="F20" s="5"/>
-      <c r="G20" s="5"/>
-      <c r="H20" s="3"/>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A21" s="3"/>
-      <c r="B21" s="3"/>
-      <c r="C21" s="3"/>
-      <c r="D21" s="3"/>
-      <c r="E21" s="3"/>
-      <c r="F21" s="5"/>
-      <c r="G21" s="5"/>
-      <c r="H21" s="3"/>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A22" s="22" t="s">
-        <v>69</v>
-      </c>
-      <c r="B22" s="23"/>
-      <c r="C22" s="23"/>
-      <c r="D22" s="23"/>
-      <c r="E22" s="23"/>
-      <c r="F22" s="23"/>
-      <c r="G22" s="23"/>
-      <c r="H22" s="24"/>
-    </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A23" s="3"/>
-      <c r="B23" s="3"/>
-      <c r="C23" s="3"/>
-      <c r="D23" s="3"/>
-      <c r="E23" s="3"/>
-      <c r="F23" s="5"/>
-      <c r="G23" s="5"/>
-      <c r="H23" s="3"/>
-    </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A24" s="3"/>
-      <c r="B24" s="3"/>
-      <c r="C24" s="3"/>
-      <c r="D24" s="3"/>
-      <c r="E24" s="3"/>
-      <c r="F24" s="5"/>
-      <c r="G24" s="5"/>
-      <c r="H24" s="3"/>
-    </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A25" s="3"/>
-      <c r="B25" s="3"/>
-      <c r="C25" s="3"/>
-      <c r="D25" s="3"/>
-      <c r="E25" s="3"/>
-      <c r="F25" s="5"/>
-      <c r="G25" s="5"/>
-      <c r="H25" s="3"/>
+      <c r="A14" s="29" t="s">
+        <v>51</v>
+      </c>
+      <c r="B14" s="30"/>
+      <c r="C14" s="30"/>
+      <c r="D14" s="30"/>
+      <c r="E14" s="30"/>
+      <c r="F14" s="30"/>
+      <c r="G14" s="30"/>
+      <c r="H14" s="31"/>
+    </row>
+    <row r="15" spans="1:8" ht="120" x14ac:dyDescent="0.25">
+      <c r="A15" s="15">
+        <v>12</v>
+      </c>
+      <c r="B15" s="35" t="s">
+        <v>87</v>
+      </c>
+      <c r="C15" s="35" t="s">
+        <v>88</v>
+      </c>
+      <c r="D15" s="35" t="s">
+        <v>89</v>
+      </c>
+      <c r="E15" s="35" t="s">
+        <v>90</v>
+      </c>
+      <c r="F15" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="G15" s="36"/>
+      <c r="H15" s="15"/>
+    </row>
+    <row r="16" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="A16" s="15">
+        <v>13</v>
+      </c>
+      <c r="B16" s="35" t="s">
+        <v>92</v>
+      </c>
+      <c r="C16" s="35" t="s">
+        <v>91</v>
+      </c>
+      <c r="D16" s="35" t="s">
+        <v>93</v>
+      </c>
+      <c r="E16" s="15" t="s">
+        <v>94</v>
+      </c>
+      <c r="F16" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="G16" s="36"/>
+      <c r="H16" s="15"/>
+    </row>
+    <row r="17" spans="1:8" ht="60" x14ac:dyDescent="0.25">
+      <c r="A17" s="15">
+        <v>14</v>
+      </c>
+      <c r="B17" s="4" t="s">
+        <v>95</v>
+      </c>
+      <c r="C17" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="D17" s="4" t="s">
+        <v>97</v>
+      </c>
+      <c r="E17" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="F17" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="G17" s="36"/>
+      <c r="H17" s="15"/>
+    </row>
+    <row r="18" spans="1:8" ht="60" x14ac:dyDescent="0.25">
+      <c r="A18" s="15">
+        <v>15</v>
+      </c>
+      <c r="B18" s="4" t="s">
+        <v>99</v>
+      </c>
+      <c r="C18" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="D18" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="E18" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="F18" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="G18" s="36"/>
+      <c r="H18" s="15"/>
+    </row>
+    <row r="19" spans="1:8" ht="60" x14ac:dyDescent="0.25">
+      <c r="A19" s="15">
+        <v>16</v>
+      </c>
+      <c r="B19" s="4" t="s">
+        <v>105</v>
+      </c>
+      <c r="C19" s="4" t="s">
+        <v>101</v>
+      </c>
+      <c r="D19" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="E19" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="F19" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="G19" s="36"/>
+      <c r="H19" s="15"/>
+    </row>
+    <row r="20" spans="1:8" ht="60" x14ac:dyDescent="0.25">
+      <c r="A20" s="15">
+        <v>17</v>
+      </c>
+      <c r="B20" s="4" t="s">
+        <v>106</v>
+      </c>
+      <c r="C20" s="4" t="s">
+        <v>102</v>
+      </c>
+      <c r="D20" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="E20" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="F20" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="G20" s="36"/>
+      <c r="H20" s="15"/>
+    </row>
+    <row r="21" spans="1:8" ht="60" x14ac:dyDescent="0.25">
+      <c r="A21" s="15">
+        <v>18</v>
+      </c>
+      <c r="B21" s="4" t="s">
+        <v>107</v>
+      </c>
+      <c r="C21" s="4" t="s">
+        <v>103</v>
+      </c>
+      <c r="D21" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="E21" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="F21" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="G21" s="36"/>
+      <c r="H21" s="15"/>
+    </row>
+    <row r="22" spans="1:8" ht="60" x14ac:dyDescent="0.25">
+      <c r="A22" s="15">
+        <v>19</v>
+      </c>
+      <c r="B22" s="4" t="s">
+        <v>108</v>
+      </c>
+      <c r="C22" s="4" t="s">
+        <v>104</v>
+      </c>
+      <c r="D22" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="E22" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="F22" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="G22" s="36"/>
+      <c r="H22" s="15"/>
+    </row>
+    <row r="23" spans="1:8" ht="60" x14ac:dyDescent="0.25">
+      <c r="A23" s="15">
+        <v>20</v>
+      </c>
+      <c r="B23" s="4" t="s">
+        <v>192</v>
+      </c>
+      <c r="C23" s="4" t="s">
+        <v>196</v>
+      </c>
+      <c r="D23" s="4" t="s">
+        <v>197</v>
+      </c>
+      <c r="E23" s="4" t="s">
+        <v>198</v>
+      </c>
+      <c r="F23" s="37" t="s">
+        <v>195</v>
+      </c>
+      <c r="G23" s="36"/>
+      <c r="H23" s="3" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" ht="120" x14ac:dyDescent="0.25">
+      <c r="A24" s="15">
+        <v>21</v>
+      </c>
+      <c r="B24" s="4" t="s">
+        <v>112</v>
+      </c>
+      <c r="C24" s="4" t="s">
+        <v>117</v>
+      </c>
+      <c r="D24" s="4" t="s">
+        <v>113</v>
+      </c>
+      <c r="E24" s="4" t="s">
+        <v>114</v>
+      </c>
+      <c r="F24" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="G24" s="36"/>
+      <c r="H24" s="15"/>
+    </row>
+    <row r="25" spans="1:8" ht="120" x14ac:dyDescent="0.25">
+      <c r="A25" s="32">
+        <v>22</v>
+      </c>
+      <c r="B25" s="33" t="s">
+        <v>115</v>
+      </c>
+      <c r="C25" s="33" t="s">
+        <v>116</v>
+      </c>
+      <c r="D25" s="33" t="s">
+        <v>118</v>
+      </c>
+      <c r="E25" s="33" t="s">
+        <v>119</v>
+      </c>
+      <c r="F25" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="G25" s="36"/>
+      <c r="H25" s="15"/>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A26" s="22" t="s">
-        <v>70</v>
-      </c>
-      <c r="B26" s="23"/>
-      <c r="C26" s="23"/>
-      <c r="D26" s="23"/>
-      <c r="E26" s="23"/>
-      <c r="F26" s="23"/>
-      <c r="G26" s="23"/>
-      <c r="H26" s="24"/>
-    </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A27" s="3"/>
-      <c r="B27" s="3"/>
-      <c r="C27" s="3"/>
-      <c r="D27" s="3"/>
-      <c r="E27" s="3"/>
-      <c r="F27" s="5"/>
+      <c r="A26" s="29" t="s">
+        <v>67</v>
+      </c>
+      <c r="B26" s="30"/>
+      <c r="C26" s="30"/>
+      <c r="D26" s="30"/>
+      <c r="E26" s="30"/>
+      <c r="F26" s="30"/>
+      <c r="G26" s="30"/>
+      <c r="H26" s="31"/>
+    </row>
+    <row r="27" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A27" s="3">
+        <v>23</v>
+      </c>
+      <c r="B27" s="4" t="s">
+        <v>128</v>
+      </c>
+      <c r="C27" s="4" t="s">
+        <v>131</v>
+      </c>
+      <c r="D27" s="4" t="s">
+        <v>129</v>
+      </c>
+      <c r="E27" s="4" t="s">
+        <v>130</v>
+      </c>
+      <c r="F27" s="6" t="s">
+        <v>20</v>
+      </c>
       <c r="G27" s="5"/>
       <c r="H27" s="3"/>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A28" s="3"/>
-      <c r="B28" s="3"/>
-      <c r="C28" s="3"/>
-      <c r="D28" s="3"/>
-      <c r="E28" s="3"/>
-      <c r="F28" s="5"/>
+    <row r="28" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="A28" s="3">
+        <v>24</v>
+      </c>
+      <c r="B28" s="4" t="s">
+        <v>132</v>
+      </c>
+      <c r="C28" s="4" t="s">
+        <v>133</v>
+      </c>
+      <c r="D28" s="4" t="s">
+        <v>134</v>
+      </c>
+      <c r="E28" s="4" t="s">
+        <v>135</v>
+      </c>
+      <c r="F28" s="6" t="s">
+        <v>20</v>
+      </c>
       <c r="G28" s="5"/>
       <c r="H28" s="3"/>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A29" s="3"/>
-      <c r="B29" s="3"/>
-      <c r="C29" s="3"/>
-      <c r="D29" s="3"/>
-      <c r="E29" s="3"/>
-      <c r="F29" s="5"/>
-      <c r="G29" s="5"/>
-      <c r="H29" s="3"/>
+    <row r="29" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="A29" s="32">
+        <v>25</v>
+      </c>
+      <c r="B29" s="32" t="s">
+        <v>136</v>
+      </c>
+      <c r="C29" s="33" t="s">
+        <v>137</v>
+      </c>
+      <c r="D29" s="33" t="s">
+        <v>139</v>
+      </c>
+      <c r="E29" s="33" t="s">
+        <v>138</v>
+      </c>
+      <c r="F29" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="G29" s="34"/>
+      <c r="H29" s="32"/>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A30" s="3"/>
-      <c r="B30" s="3"/>
-      <c r="C30" s="3"/>
-      <c r="D30" s="3"/>
-      <c r="E30" s="3"/>
-      <c r="F30" s="5"/>
-      <c r="G30" s="5"/>
-      <c r="H30" s="3"/>
-    </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A31" s="3"/>
-      <c r="B31" s="3"/>
-      <c r="C31" s="3"/>
-      <c r="D31" s="3"/>
-      <c r="E31" s="3"/>
-      <c r="F31" s="5"/>
+      <c r="A30" s="29" t="s">
+        <v>61</v>
+      </c>
+      <c r="B30" s="30"/>
+      <c r="C30" s="30"/>
+      <c r="D30" s="30"/>
+      <c r="E30" s="30"/>
+      <c r="F30" s="30"/>
+      <c r="G30" s="30"/>
+      <c r="H30" s="31"/>
+    </row>
+    <row r="31" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="A31" s="3">
+        <v>26</v>
+      </c>
+      <c r="B31" s="4" t="s">
+        <v>152</v>
+      </c>
+      <c r="C31" s="4" t="s">
+        <v>153</v>
+      </c>
+      <c r="D31" s="4" t="s">
+        <v>172</v>
+      </c>
+      <c r="E31" s="4" t="s">
+        <v>177</v>
+      </c>
+      <c r="F31" s="6" t="s">
+        <v>20</v>
+      </c>
       <c r="G31" s="5"/>
       <c r="H31" s="3"/>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A32" s="3"/>
-      <c r="B32" s="3"/>
-      <c r="C32" s="3"/>
-      <c r="D32" s="3"/>
-      <c r="E32" s="3"/>
-      <c r="F32" s="5"/>
+    <row r="32" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="A32" s="3">
+        <v>27</v>
+      </c>
+      <c r="B32" s="4" t="s">
+        <v>152</v>
+      </c>
+      <c r="C32" s="4" t="s">
+        <v>154</v>
+      </c>
+      <c r="D32" s="4" t="s">
+        <v>173</v>
+      </c>
+      <c r="E32" s="4" t="s">
+        <v>180</v>
+      </c>
+      <c r="F32" s="6" t="s">
+        <v>20</v>
+      </c>
       <c r="G32" s="5"/>
       <c r="H32" s="3"/>
     </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A33" s="3"/>
-      <c r="B33" s="3"/>
-      <c r="C33" s="3"/>
-      <c r="D33" s="3"/>
-      <c r="E33" s="3"/>
-      <c r="F33" s="5"/>
+    <row r="33" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="A33" s="3">
+        <v>28</v>
+      </c>
+      <c r="B33" s="4" t="s">
+        <v>152</v>
+      </c>
+      <c r="C33" s="4" t="s">
+        <v>155</v>
+      </c>
+      <c r="D33" s="4" t="s">
+        <v>174</v>
+      </c>
+      <c r="E33" s="4" t="s">
+        <v>178</v>
+      </c>
+      <c r="F33" s="6" t="s">
+        <v>20</v>
+      </c>
       <c r="G33" s="5"/>
       <c r="H33" s="3"/>
     </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A34" s="3"/>
-      <c r="B34" s="3"/>
-      <c r="C34" s="3"/>
-      <c r="D34" s="3"/>
-      <c r="E34" s="3"/>
-      <c r="F34" s="5"/>
+    <row r="34" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="A34" s="3">
+        <v>29</v>
+      </c>
+      <c r="B34" s="4" t="s">
+        <v>152</v>
+      </c>
+      <c r="C34" s="4" t="s">
+        <v>156</v>
+      </c>
+      <c r="D34" s="4" t="s">
+        <v>175</v>
+      </c>
+      <c r="E34" s="4" t="s">
+        <v>179</v>
+      </c>
+      <c r="F34" s="6" t="s">
+        <v>20</v>
+      </c>
       <c r="G34" s="5"/>
       <c r="H34" s="3"/>
     </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A35" s="3"/>
-      <c r="B35" s="3"/>
-      <c r="C35" s="3"/>
-      <c r="D35" s="3"/>
-      <c r="E35" s="3"/>
-      <c r="F35" s="5"/>
+    <row r="35" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="A35" s="3">
+        <v>30</v>
+      </c>
+      <c r="B35" s="4" t="s">
+        <v>152</v>
+      </c>
+      <c r="C35" s="4" t="s">
+        <v>157</v>
+      </c>
+      <c r="D35" s="4" t="s">
+        <v>176</v>
+      </c>
+      <c r="E35" s="4" t="s">
+        <v>181</v>
+      </c>
+      <c r="F35" s="6" t="s">
+        <v>20</v>
+      </c>
       <c r="G35" s="5"/>
       <c r="H35" s="3"/>
     </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A36" s="3"/>
-      <c r="B36" s="3"/>
-      <c r="C36" s="3"/>
-      <c r="D36" s="3"/>
-      <c r="E36" s="3"/>
-      <c r="F36" s="5"/>
+    <row r="36" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="A36" s="3">
+        <v>31</v>
+      </c>
+      <c r="B36" s="4" t="s">
+        <v>152</v>
+      </c>
+      <c r="C36" s="4" t="s">
+        <v>159</v>
+      </c>
+      <c r="D36" s="4" t="s">
+        <v>170</v>
+      </c>
+      <c r="E36" s="4" t="s">
+        <v>171</v>
+      </c>
+      <c r="F36" s="6" t="s">
+        <v>20</v>
+      </c>
       <c r="G36" s="5"/>
       <c r="H36" s="3"/>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A37" s="3"/>
-      <c r="B37" s="3"/>
-      <c r="C37" s="3"/>
-      <c r="D37" s="3"/>
-      <c r="E37" s="3"/>
-      <c r="F37" s="5"/>
-      <c r="G37" s="5"/>
-      <c r="H37" s="3"/>
-    </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A38" s="3"/>
-      <c r="B38" s="3"/>
-      <c r="C38" s="3"/>
-      <c r="D38" s="3"/>
-      <c r="E38" s="3"/>
-      <c r="F38" s="5"/>
+      <c r="A37" s="29" t="s">
+        <v>68</v>
+      </c>
+      <c r="B37" s="30"/>
+      <c r="C37" s="30"/>
+      <c r="D37" s="30"/>
+      <c r="E37" s="30"/>
+      <c r="F37" s="30"/>
+      <c r="G37" s="30"/>
+      <c r="H37" s="31"/>
+    </row>
+    <row r="38" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A38" s="3">
+        <v>32</v>
+      </c>
+      <c r="B38" s="4" t="s">
+        <v>140</v>
+      </c>
+      <c r="C38" s="4" t="s">
+        <v>143</v>
+      </c>
+      <c r="D38" s="4" t="s">
+        <v>146</v>
+      </c>
+      <c r="E38" s="4" t="s">
+        <v>148</v>
+      </c>
+      <c r="F38" s="6" t="s">
+        <v>20</v>
+      </c>
       <c r="G38" s="5"/>
       <c r="H38" s="3"/>
     </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A39" s="3"/>
-      <c r="B39" s="3"/>
-      <c r="C39" s="3"/>
-      <c r="D39" s="3"/>
-      <c r="E39" s="3"/>
-      <c r="F39" s="5"/>
+    <row r="39" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A39" s="3">
+        <v>33</v>
+      </c>
+      <c r="B39" s="4" t="s">
+        <v>141</v>
+      </c>
+      <c r="C39" s="4" t="s">
+        <v>144</v>
+      </c>
+      <c r="D39" s="4" t="s">
+        <v>147</v>
+      </c>
+      <c r="E39" s="4" t="s">
+        <v>149</v>
+      </c>
+      <c r="F39" s="6" t="s">
+        <v>20</v>
+      </c>
       <c r="G39" s="5"/>
       <c r="H39" s="3"/>
     </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A40" s="3"/>
-      <c r="B40" s="3"/>
-      <c r="C40" s="3"/>
-      <c r="D40" s="3"/>
-      <c r="E40" s="3"/>
-      <c r="F40" s="5"/>
+    <row r="40" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A40" s="3">
+        <v>34</v>
+      </c>
+      <c r="B40" s="4" t="s">
+        <v>142</v>
+      </c>
+      <c r="C40" s="4" t="s">
+        <v>145</v>
+      </c>
+      <c r="D40" s="4" t="s">
+        <v>150</v>
+      </c>
+      <c r="E40" s="4" t="s">
+        <v>151</v>
+      </c>
+      <c r="F40" s="6" t="s">
+        <v>20</v>
+      </c>
       <c r="G40" s="5"/>
       <c r="H40" s="3"/>
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A41" s="3"/>
-      <c r="B41" s="3"/>
-      <c r="C41" s="3"/>
-      <c r="D41" s="3"/>
-      <c r="E41" s="3"/>
-      <c r="F41" s="5"/>
-      <c r="G41" s="5"/>
-      <c r="H41" s="3"/>
-    </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A42" s="3"/>
-      <c r="B42" s="3"/>
-      <c r="C42" s="3"/>
-      <c r="D42" s="3"/>
-      <c r="E42" s="3"/>
-      <c r="F42" s="5"/>
+      <c r="A41" s="29" t="s">
+        <v>69</v>
+      </c>
+      <c r="B41" s="30"/>
+      <c r="C41" s="30"/>
+      <c r="D41" s="30"/>
+      <c r="E41" s="30"/>
+      <c r="F41" s="30"/>
+      <c r="G41" s="30"/>
+      <c r="H41" s="31"/>
+    </row>
+    <row r="42" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A42" s="3">
+        <v>35</v>
+      </c>
+      <c r="B42" s="4" t="s">
+        <v>160</v>
+      </c>
+      <c r="C42" s="4" t="s">
+        <v>165</v>
+      </c>
+      <c r="D42" s="4" t="s">
+        <v>182</v>
+      </c>
+      <c r="E42" s="3" t="s">
+        <v>186</v>
+      </c>
+      <c r="F42" s="6" t="s">
+        <v>20</v>
+      </c>
       <c r="G42" s="5"/>
       <c r="H42" s="3"/>
     </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A43" s="3"/>
-      <c r="B43" s="3"/>
-      <c r="C43" s="3"/>
-      <c r="D43" s="3"/>
-      <c r="E43" s="3"/>
-      <c r="F43" s="5"/>
+    <row r="43" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A43" s="3">
+        <v>36</v>
+      </c>
+      <c r="B43" s="4" t="s">
+        <v>161</v>
+      </c>
+      <c r="C43" s="4" t="s">
+        <v>166</v>
+      </c>
+      <c r="D43" s="4" t="s">
+        <v>184</v>
+      </c>
+      <c r="E43" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="F43" s="6" t="s">
+        <v>20</v>
+      </c>
       <c r="G43" s="5"/>
       <c r="H43" s="3"/>
     </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A44" s="3"/>
-      <c r="B44" s="3"/>
-      <c r="C44" s="3"/>
-      <c r="D44" s="3"/>
-      <c r="E44" s="3"/>
-      <c r="F44" s="5"/>
+    <row r="44" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A44" s="3">
+        <v>37</v>
+      </c>
+      <c r="B44" s="4" t="s">
+        <v>162</v>
+      </c>
+      <c r="C44" s="4" t="s">
+        <v>167</v>
+      </c>
+      <c r="D44" s="4" t="s">
+        <v>183</v>
+      </c>
+      <c r="E44" s="3" t="s">
+        <v>189</v>
+      </c>
+      <c r="F44" s="6" t="s">
+        <v>20</v>
+      </c>
       <c r="G44" s="5"/>
       <c r="H44" s="3"/>
     </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A45" s="3"/>
-      <c r="B45" s="3"/>
-      <c r="C45" s="3"/>
-      <c r="D45" s="3"/>
-      <c r="E45" s="3"/>
-      <c r="F45" s="5"/>
+    <row r="45" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A45" s="3">
+        <v>38</v>
+      </c>
+      <c r="B45" s="4" t="s">
+        <v>163</v>
+      </c>
+      <c r="C45" s="4" t="s">
+        <v>168</v>
+      </c>
+      <c r="D45" s="4" t="s">
+        <v>185</v>
+      </c>
+      <c r="E45" s="3" t="s">
+        <v>188</v>
+      </c>
+      <c r="F45" s="6" t="s">
+        <v>20</v>
+      </c>
       <c r="G45" s="5"/>
       <c r="H45" s="3"/>
     </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A46" s="3"/>
-      <c r="B46" s="3"/>
-      <c r="C46" s="3"/>
-      <c r="D46" s="3"/>
-      <c r="E46" s="3"/>
-      <c r="F46" s="5"/>
+    <row r="46" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A46" s="3">
+        <v>39</v>
+      </c>
+      <c r="B46" s="4" t="s">
+        <v>164</v>
+      </c>
+      <c r="C46" s="4" t="s">
+        <v>169</v>
+      </c>
+      <c r="D46" s="4" t="s">
+        <v>191</v>
+      </c>
+      <c r="E46" s="3" t="s">
+        <v>190</v>
+      </c>
+      <c r="F46" s="6" t="s">
+        <v>20</v>
+      </c>
       <c r="G46" s="5"/>
       <c r="H46" s="3"/>
     </row>
@@ -2952,20 +4169,170 @@
       <c r="G83" s="5"/>
       <c r="H83" s="3"/>
     </row>
+    <row r="84" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A84" s="3"/>
+      <c r="B84" s="3"/>
+      <c r="C84" s="3"/>
+      <c r="D84" s="3"/>
+      <c r="E84" s="3"/>
+      <c r="F84" s="5"/>
+      <c r="G84" s="5"/>
+      <c r="H84" s="3"/>
+    </row>
+    <row r="85" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A85" s="3"/>
+      <c r="B85" s="3"/>
+      <c r="C85" s="3"/>
+      <c r="D85" s="3"/>
+      <c r="E85" s="3"/>
+      <c r="F85" s="5"/>
+      <c r="G85" s="5"/>
+      <c r="H85" s="3"/>
+    </row>
+    <row r="86" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A86" s="3"/>
+      <c r="B86" s="3"/>
+      <c r="C86" s="3"/>
+      <c r="D86" s="3"/>
+      <c r="E86" s="3"/>
+      <c r="F86" s="5"/>
+      <c r="G86" s="5"/>
+      <c r="H86" s="3"/>
+    </row>
+    <row r="87" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A87" s="3"/>
+      <c r="B87" s="3"/>
+      <c r="C87" s="3"/>
+      <c r="D87" s="3"/>
+      <c r="E87" s="3"/>
+      <c r="F87" s="5"/>
+      <c r="G87" s="5"/>
+      <c r="H87" s="3"/>
+    </row>
+    <row r="88" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A88" s="3"/>
+      <c r="B88" s="3"/>
+      <c r="C88" s="3"/>
+      <c r="D88" s="3"/>
+      <c r="E88" s="3"/>
+      <c r="F88" s="5"/>
+      <c r="G88" s="5"/>
+      <c r="H88" s="3"/>
+    </row>
+    <row r="89" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A89" s="3"/>
+      <c r="B89" s="3"/>
+      <c r="C89" s="3"/>
+      <c r="D89" s="3"/>
+      <c r="E89" s="3"/>
+      <c r="F89" s="5"/>
+      <c r="G89" s="5"/>
+      <c r="H89" s="3"/>
+    </row>
+    <row r="90" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A90" s="3"/>
+      <c r="B90" s="3"/>
+      <c r="C90" s="3"/>
+      <c r="D90" s="3"/>
+      <c r="E90" s="3"/>
+      <c r="F90" s="5"/>
+      <c r="G90" s="5"/>
+      <c r="H90" s="3"/>
+    </row>
+    <row r="91" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A91" s="3"/>
+      <c r="B91" s="3"/>
+      <c r="C91" s="3"/>
+      <c r="D91" s="3"/>
+      <c r="E91" s="3"/>
+      <c r="F91" s="5"/>
+      <c r="G91" s="5"/>
+      <c r="H91" s="3"/>
+    </row>
+    <row r="92" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A92" s="3"/>
+      <c r="B92" s="3"/>
+      <c r="C92" s="3"/>
+      <c r="D92" s="3"/>
+      <c r="E92" s="3"/>
+      <c r="F92" s="5"/>
+      <c r="G92" s="5"/>
+      <c r="H92" s="3"/>
+    </row>
+    <row r="93" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A93" s="3"/>
+      <c r="B93" s="3"/>
+      <c r="C93" s="3"/>
+      <c r="D93" s="3"/>
+      <c r="E93" s="3"/>
+      <c r="F93" s="5"/>
+      <c r="G93" s="5"/>
+      <c r="H93" s="3"/>
+    </row>
+    <row r="94" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A94" s="3"/>
+      <c r="B94" s="3"/>
+      <c r="C94" s="3"/>
+      <c r="D94" s="3"/>
+      <c r="E94" s="3"/>
+      <c r="F94" s="5"/>
+      <c r="G94" s="5"/>
+      <c r="H94" s="3"/>
+    </row>
+    <row r="95" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A95" s="3"/>
+      <c r="B95" s="3"/>
+      <c r="C95" s="3"/>
+      <c r="D95" s="3"/>
+      <c r="E95" s="3"/>
+      <c r="F95" s="5"/>
+      <c r="G95" s="5"/>
+      <c r="H95" s="3"/>
+    </row>
+    <row r="96" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A96" s="3"/>
+      <c r="B96" s="3"/>
+      <c r="C96" s="3"/>
+      <c r="D96" s="3"/>
+      <c r="E96" s="3"/>
+      <c r="F96" s="5"/>
+      <c r="G96" s="5"/>
+      <c r="H96" s="3"/>
+    </row>
+    <row r="97" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A97" s="3"/>
+      <c r="B97" s="3"/>
+      <c r="C97" s="3"/>
+      <c r="D97" s="3"/>
+      <c r="E97" s="3"/>
+      <c r="F97" s="5"/>
+      <c r="G97" s="5"/>
+      <c r="H97" s="3"/>
+    </row>
+    <row r="98" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A98" s="3"/>
+      <c r="B98" s="3"/>
+      <c r="C98" s="3"/>
+      <c r="D98" s="3"/>
+      <c r="E98" s="3"/>
+      <c r="F98" s="5"/>
+      <c r="G98" s="5"/>
+      <c r="H98" s="3"/>
+    </row>
   </sheetData>
   <mergeCells count="6">
+    <mergeCell ref="A41:H41"/>
     <mergeCell ref="A2:H2"/>
-    <mergeCell ref="A10:H10"/>
     <mergeCell ref="A14:H14"/>
-    <mergeCell ref="A18:H18"/>
-    <mergeCell ref="A22:H22"/>
     <mergeCell ref="A26:H26"/>
+    <mergeCell ref="A30:H30"/>
+    <mergeCell ref="A37:H37"/>
   </mergeCells>
   <dataValidations count="2">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G3" xr:uid="{9E7A5853-1C00-445C-9290-798981E423AE}">
       <formula1>"A - High, B - Medium, C - Low, None"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G4:G9 G11:G13 G15:G17 G19:G21 G23:G25 G27:G83" xr:uid="{1D89D116-AAC3-4E50-911F-ACA0B7F5AAEC}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G42:G98 G27:G29 G31:G36 G38:G40 G4:G13 G15:G25" xr:uid="{1D89D116-AAC3-4E50-911F-ACA0B7F5AAEC}">
       <formula1>"A- High, B - Medium, C - Low, None"</formula1>
     </dataValidation>
   </dataValidations>
@@ -2978,7 +4345,7 @@
   <dimension ref="A1:B591"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H17" sqref="H17"/>
+      <selection activeCell="N27" sqref="N27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2996,7 +4363,9 @@
       </c>
     </row>
     <row r="2" spans="1:2" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="7"/>
+      <c r="A2" s="7">
+        <v>1</v>
+      </c>
     </row>
     <row r="3" spans="1:2" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="7"/>
@@ -3047,7 +4416,9 @@
       <c r="A18" s="7"/>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A19" s="7"/>
+      <c r="A19" s="7">
+        <v>2</v>
+      </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A20" s="7"/>
@@ -4764,5 +6135,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
fix: fill-in the severity of each test case
</commit_message>
<xml_diff>
--- a/test_cases/Book Catalog - Test Cases.xlsx
+++ b/test_cases/Book Catalog - Test Cases.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\PROGRAMMING_HABIT\bookcatalog-automation\test_cases\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{20C8B178-147E-47BC-AD88-CF34C9AB92A2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{966BF1A6-1F47-4960-9780-701277857AAA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Title" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="342" uniqueCount="203">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="379" uniqueCount="203">
   <si>
     <t>Application name</t>
   </si>
@@ -1133,7 +1133,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="38">
+  <cellXfs count="37">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1164,17 +1164,20 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="10" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -1183,9 +1186,6 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
@@ -1203,6 +1203,21 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
@@ -1211,24 +1226,6 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="10" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1782,370 +1779,370 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z24"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <selection activeCell="I33" sqref="I33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="16" t="s">
+      <c r="A1" s="32" t="s">
         <v>29</v>
       </c>
-      <c r="B1" s="16"/>
-      <c r="C1" s="16"/>
-      <c r="D1" s="16"/>
-      <c r="E1" s="16"/>
-      <c r="F1" s="16"/>
-      <c r="G1" s="16"/>
-      <c r="H1" s="16"/>
-      <c r="I1" s="16"/>
-      <c r="J1" s="16"/>
-      <c r="K1" s="16"/>
-      <c r="L1" s="16"/>
-      <c r="M1" s="16"/>
-      <c r="N1" s="16"/>
-      <c r="O1" s="16"/>
-      <c r="P1" s="16"/>
-      <c r="Q1" s="16"/>
-      <c r="R1" s="16"/>
-      <c r="S1" s="16"/>
-      <c r="T1" s="16"/>
-      <c r="U1" s="16"/>
-      <c r="V1" s="16"/>
-      <c r="W1" s="16"/>
-      <c r="X1" s="16"/>
-      <c r="Y1" s="16"/>
-      <c r="Z1" s="16"/>
+      <c r="B1" s="32"/>
+      <c r="C1" s="32"/>
+      <c r="D1" s="32"/>
+      <c r="E1" s="32"/>
+      <c r="F1" s="32"/>
+      <c r="G1" s="32"/>
+      <c r="H1" s="32"/>
+      <c r="I1" s="32"/>
+      <c r="J1" s="32"/>
+      <c r="K1" s="32"/>
+      <c r="L1" s="32"/>
+      <c r="M1" s="32"/>
+      <c r="N1" s="32"/>
+      <c r="O1" s="32"/>
+      <c r="P1" s="32"/>
+      <c r="Q1" s="32"/>
+      <c r="R1" s="32"/>
+      <c r="S1" s="32"/>
+      <c r="T1" s="32"/>
+      <c r="U1" s="32"/>
+      <c r="V1" s="32"/>
+      <c r="W1" s="32"/>
+      <c r="X1" s="32"/>
+      <c r="Y1" s="32"/>
+      <c r="Z1" s="32"/>
     </row>
     <row r="2" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="16"/>
-      <c r="B2" s="16"/>
-      <c r="C2" s="16"/>
-      <c r="D2" s="16"/>
-      <c r="E2" s="16"/>
-      <c r="F2" s="16"/>
-      <c r="G2" s="16"/>
-      <c r="H2" s="16"/>
-      <c r="I2" s="16"/>
-      <c r="J2" s="16"/>
-      <c r="K2" s="16"/>
-      <c r="L2" s="16"/>
-      <c r="M2" s="16"/>
-      <c r="N2" s="16"/>
-      <c r="O2" s="16"/>
-      <c r="P2" s="16"/>
-      <c r="Q2" s="16"/>
-      <c r="R2" s="16"/>
-      <c r="S2" s="16"/>
-      <c r="T2" s="16"/>
-      <c r="U2" s="16"/>
-      <c r="V2" s="16"/>
-      <c r="W2" s="16"/>
-      <c r="X2" s="16"/>
-      <c r="Y2" s="16"/>
-      <c r="Z2" s="16"/>
+      <c r="A2" s="32"/>
+      <c r="B2" s="32"/>
+      <c r="C2" s="32"/>
+      <c r="D2" s="32"/>
+      <c r="E2" s="32"/>
+      <c r="F2" s="32"/>
+      <c r="G2" s="32"/>
+      <c r="H2" s="32"/>
+      <c r="I2" s="32"/>
+      <c r="J2" s="32"/>
+      <c r="K2" s="32"/>
+      <c r="L2" s="32"/>
+      <c r="M2" s="32"/>
+      <c r="N2" s="32"/>
+      <c r="O2" s="32"/>
+      <c r="P2" s="32"/>
+      <c r="Q2" s="32"/>
+      <c r="R2" s="32"/>
+      <c r="S2" s="32"/>
+      <c r="T2" s="32"/>
+      <c r="U2" s="32"/>
+      <c r="V2" s="32"/>
+      <c r="W2" s="32"/>
+      <c r="X2" s="32"/>
+      <c r="Y2" s="32"/>
+      <c r="Z2" s="32"/>
     </row>
     <row r="3" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="16"/>
-      <c r="B3" s="16"/>
-      <c r="C3" s="16"/>
-      <c r="D3" s="16"/>
-      <c r="E3" s="16"/>
-      <c r="F3" s="16"/>
-      <c r="G3" s="16"/>
-      <c r="H3" s="16"/>
-      <c r="I3" s="16"/>
-      <c r="J3" s="16"/>
-      <c r="K3" s="16"/>
-      <c r="L3" s="16"/>
-      <c r="M3" s="16"/>
-      <c r="N3" s="16"/>
-      <c r="O3" s="16"/>
-      <c r="P3" s="16"/>
-      <c r="Q3" s="16"/>
-      <c r="R3" s="16"/>
-      <c r="S3" s="16"/>
-      <c r="T3" s="16"/>
-      <c r="U3" s="16"/>
-      <c r="V3" s="16"/>
-      <c r="W3" s="16"/>
-      <c r="X3" s="16"/>
-      <c r="Y3" s="16"/>
-      <c r="Z3" s="16"/>
+      <c r="A3" s="32"/>
+      <c r="B3" s="32"/>
+      <c r="C3" s="32"/>
+      <c r="D3" s="32"/>
+      <c r="E3" s="32"/>
+      <c r="F3" s="32"/>
+      <c r="G3" s="32"/>
+      <c r="H3" s="32"/>
+      <c r="I3" s="32"/>
+      <c r="J3" s="32"/>
+      <c r="K3" s="32"/>
+      <c r="L3" s="32"/>
+      <c r="M3" s="32"/>
+      <c r="N3" s="32"/>
+      <c r="O3" s="32"/>
+      <c r="P3" s="32"/>
+      <c r="Q3" s="32"/>
+      <c r="R3" s="32"/>
+      <c r="S3" s="32"/>
+      <c r="T3" s="32"/>
+      <c r="U3" s="32"/>
+      <c r="V3" s="32"/>
+      <c r="W3" s="32"/>
+      <c r="X3" s="32"/>
+      <c r="Y3" s="32"/>
+      <c r="Z3" s="32"/>
     </row>
     <row r="4" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="16"/>
-      <c r="B4" s="16"/>
-      <c r="C4" s="16"/>
-      <c r="D4" s="16"/>
-      <c r="E4" s="16"/>
-      <c r="F4" s="16"/>
-      <c r="G4" s="16"/>
-      <c r="H4" s="16"/>
-      <c r="I4" s="16"/>
-      <c r="J4" s="16"/>
-      <c r="K4" s="16"/>
-      <c r="L4" s="16"/>
-      <c r="M4" s="16"/>
-      <c r="N4" s="16"/>
-      <c r="O4" s="16"/>
-      <c r="P4" s="16"/>
-      <c r="Q4" s="16"/>
-      <c r="R4" s="16"/>
-      <c r="S4" s="16"/>
-      <c r="T4" s="16"/>
-      <c r="U4" s="16"/>
-      <c r="V4" s="16"/>
-      <c r="W4" s="16"/>
-      <c r="X4" s="16"/>
-      <c r="Y4" s="16"/>
-      <c r="Z4" s="16"/>
+      <c r="A4" s="32"/>
+      <c r="B4" s="32"/>
+      <c r="C4" s="32"/>
+      <c r="D4" s="32"/>
+      <c r="E4" s="32"/>
+      <c r="F4" s="32"/>
+      <c r="G4" s="32"/>
+      <c r="H4" s="32"/>
+      <c r="I4" s="32"/>
+      <c r="J4" s="32"/>
+      <c r="K4" s="32"/>
+      <c r="L4" s="32"/>
+      <c r="M4" s="32"/>
+      <c r="N4" s="32"/>
+      <c r="O4" s="32"/>
+      <c r="P4" s="32"/>
+      <c r="Q4" s="32"/>
+      <c r="R4" s="32"/>
+      <c r="S4" s="32"/>
+      <c r="T4" s="32"/>
+      <c r="U4" s="32"/>
+      <c r="V4" s="32"/>
+      <c r="W4" s="32"/>
+      <c r="X4" s="32"/>
+      <c r="Y4" s="32"/>
+      <c r="Z4" s="32"/>
     </row>
     <row r="5" spans="1:26" ht="3" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="16"/>
-      <c r="B5" s="16"/>
-      <c r="C5" s="16"/>
-      <c r="D5" s="16"/>
-      <c r="E5" s="16"/>
-      <c r="F5" s="16"/>
-      <c r="G5" s="16"/>
-      <c r="H5" s="16"/>
-      <c r="I5" s="16"/>
-      <c r="J5" s="16"/>
-      <c r="K5" s="16"/>
-      <c r="L5" s="16"/>
-      <c r="M5" s="16"/>
-      <c r="N5" s="16"/>
-      <c r="O5" s="16"/>
-      <c r="P5" s="16"/>
-      <c r="Q5" s="16"/>
-      <c r="R5" s="16"/>
-      <c r="S5" s="16"/>
-      <c r="T5" s="16"/>
-      <c r="U5" s="16"/>
-      <c r="V5" s="16"/>
-      <c r="W5" s="16"/>
-      <c r="X5" s="16"/>
-      <c r="Y5" s="16"/>
-      <c r="Z5" s="16"/>
+      <c r="A5" s="32"/>
+      <c r="B5" s="32"/>
+      <c r="C5" s="32"/>
+      <c r="D5" s="32"/>
+      <c r="E5" s="32"/>
+      <c r="F5" s="32"/>
+      <c r="G5" s="32"/>
+      <c r="H5" s="32"/>
+      <c r="I5" s="32"/>
+      <c r="J5" s="32"/>
+      <c r="K5" s="32"/>
+      <c r="L5" s="32"/>
+      <c r="M5" s="32"/>
+      <c r="N5" s="32"/>
+      <c r="O5" s="32"/>
+      <c r="P5" s="32"/>
+      <c r="Q5" s="32"/>
+      <c r="R5" s="32"/>
+      <c r="S5" s="32"/>
+      <c r="T5" s="32"/>
+      <c r="U5" s="32"/>
+      <c r="V5" s="32"/>
+      <c r="W5" s="32"/>
+      <c r="X5" s="32"/>
+      <c r="Y5" s="32"/>
+      <c r="Z5" s="32"/>
     </row>
     <row r="6" spans="1:26" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="16"/>
-      <c r="B6" s="16"/>
-      <c r="C6" s="16"/>
-      <c r="D6" s="16"/>
-      <c r="E6" s="16"/>
-      <c r="F6" s="16"/>
-      <c r="G6" s="16"/>
-      <c r="H6" s="16"/>
-      <c r="I6" s="16"/>
-      <c r="J6" s="16"/>
-      <c r="K6" s="16"/>
-      <c r="L6" s="16"/>
-      <c r="M6" s="16"/>
-      <c r="N6" s="16"/>
-      <c r="O6" s="16"/>
-      <c r="P6" s="16"/>
-      <c r="Q6" s="16"/>
-      <c r="R6" s="16"/>
-      <c r="S6" s="16"/>
-      <c r="T6" s="16"/>
-      <c r="U6" s="16"/>
-      <c r="V6" s="16"/>
-      <c r="W6" s="16"/>
-      <c r="X6" s="16"/>
-      <c r="Y6" s="16"/>
-      <c r="Z6" s="16"/>
+      <c r="A6" s="32"/>
+      <c r="B6" s="32"/>
+      <c r="C6" s="32"/>
+      <c r="D6" s="32"/>
+      <c r="E6" s="32"/>
+      <c r="F6" s="32"/>
+      <c r="G6" s="32"/>
+      <c r="H6" s="32"/>
+      <c r="I6" s="32"/>
+      <c r="J6" s="32"/>
+      <c r="K6" s="32"/>
+      <c r="L6" s="32"/>
+      <c r="M6" s="32"/>
+      <c r="N6" s="32"/>
+      <c r="O6" s="32"/>
+      <c r="P6" s="32"/>
+      <c r="Q6" s="32"/>
+      <c r="R6" s="32"/>
+      <c r="S6" s="32"/>
+      <c r="T6" s="32"/>
+      <c r="U6" s="32"/>
+      <c r="V6" s="32"/>
+      <c r="W6" s="32"/>
+      <c r="X6" s="32"/>
+      <c r="Y6" s="32"/>
+      <c r="Z6" s="32"/>
     </row>
     <row r="7" spans="1:26" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="16"/>
-      <c r="B7" s="16"/>
-      <c r="C7" s="16"/>
-      <c r="D7" s="16"/>
-      <c r="E7" s="16"/>
-      <c r="F7" s="16"/>
-      <c r="G7" s="16"/>
-      <c r="H7" s="16"/>
-      <c r="I7" s="16"/>
-      <c r="J7" s="16"/>
-      <c r="K7" s="16"/>
-      <c r="L7" s="16"/>
-      <c r="M7" s="16"/>
-      <c r="N7" s="16"/>
-      <c r="O7" s="16"/>
-      <c r="P7" s="16"/>
-      <c r="Q7" s="16"/>
-      <c r="R7" s="16"/>
-      <c r="S7" s="16"/>
-      <c r="T7" s="16"/>
-      <c r="U7" s="16"/>
-      <c r="V7" s="16"/>
-      <c r="W7" s="16"/>
-      <c r="X7" s="16"/>
-      <c r="Y7" s="16"/>
-      <c r="Z7" s="16"/>
+      <c r="A7" s="32"/>
+      <c r="B7" s="32"/>
+      <c r="C7" s="32"/>
+      <c r="D7" s="32"/>
+      <c r="E7" s="32"/>
+      <c r="F7" s="32"/>
+      <c r="G7" s="32"/>
+      <c r="H7" s="32"/>
+      <c r="I7" s="32"/>
+      <c r="J7" s="32"/>
+      <c r="K7" s="32"/>
+      <c r="L7" s="32"/>
+      <c r="M7" s="32"/>
+      <c r="N7" s="32"/>
+      <c r="O7" s="32"/>
+      <c r="P7" s="32"/>
+      <c r="Q7" s="32"/>
+      <c r="R7" s="32"/>
+      <c r="S7" s="32"/>
+      <c r="T7" s="32"/>
+      <c r="U7" s="32"/>
+      <c r="V7" s="32"/>
+      <c r="W7" s="32"/>
+      <c r="X7" s="32"/>
+      <c r="Y7" s="32"/>
+      <c r="Z7" s="32"/>
     </row>
     <row r="8" spans="1:26" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="16"/>
-      <c r="B8" s="16"/>
-      <c r="C8" s="16"/>
-      <c r="D8" s="16"/>
-      <c r="E8" s="16"/>
-      <c r="F8" s="16"/>
-      <c r="G8" s="16"/>
-      <c r="H8" s="16"/>
-      <c r="I8" s="16"/>
-      <c r="J8" s="16"/>
-      <c r="K8" s="16"/>
-      <c r="L8" s="16"/>
-      <c r="M8" s="16"/>
-      <c r="N8" s="16"/>
-      <c r="O8" s="16"/>
-      <c r="P8" s="16"/>
-      <c r="Q8" s="16"/>
-      <c r="R8" s="16"/>
-      <c r="S8" s="16"/>
-      <c r="T8" s="16"/>
-      <c r="U8" s="16"/>
-      <c r="V8" s="16"/>
-      <c r="W8" s="16"/>
-      <c r="X8" s="16"/>
-      <c r="Y8" s="16"/>
-      <c r="Z8" s="16"/>
+      <c r="A8" s="32"/>
+      <c r="B8" s="32"/>
+      <c r="C8" s="32"/>
+      <c r="D8" s="32"/>
+      <c r="E8" s="32"/>
+      <c r="F8" s="32"/>
+      <c r="G8" s="32"/>
+      <c r="H8" s="32"/>
+      <c r="I8" s="32"/>
+      <c r="J8" s="32"/>
+      <c r="K8" s="32"/>
+      <c r="L8" s="32"/>
+      <c r="M8" s="32"/>
+      <c r="N8" s="32"/>
+      <c r="O8" s="32"/>
+      <c r="P8" s="32"/>
+      <c r="Q8" s="32"/>
+      <c r="R8" s="32"/>
+      <c r="S8" s="32"/>
+      <c r="T8" s="32"/>
+      <c r="U8" s="32"/>
+      <c r="V8" s="32"/>
+      <c r="W8" s="32"/>
+      <c r="X8" s="32"/>
+      <c r="Y8" s="32"/>
+      <c r="Z8" s="32"/>
     </row>
     <row r="9" spans="1:26" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="16"/>
-      <c r="B9" s="16"/>
-      <c r="C9" s="16"/>
-      <c r="D9" s="16"/>
-      <c r="E9" s="16"/>
-      <c r="F9" s="16"/>
-      <c r="G9" s="16"/>
-      <c r="H9" s="16"/>
-      <c r="I9" s="16"/>
-      <c r="J9" s="16"/>
-      <c r="K9" s="16"/>
-      <c r="L9" s="16"/>
-      <c r="M9" s="16"/>
-      <c r="N9" s="16"/>
-      <c r="O9" s="16"/>
-      <c r="P9" s="16"/>
-      <c r="Q9" s="16"/>
-      <c r="R9" s="16"/>
-      <c r="S9" s="16"/>
-      <c r="T9" s="16"/>
-      <c r="U9" s="16"/>
-      <c r="V9" s="16"/>
-      <c r="W9" s="16"/>
-      <c r="X9" s="16"/>
-      <c r="Y9" s="16"/>
-      <c r="Z9" s="16"/>
+      <c r="A9" s="32"/>
+      <c r="B9" s="32"/>
+      <c r="C9" s="32"/>
+      <c r="D9" s="32"/>
+      <c r="E9" s="32"/>
+      <c r="F9" s="32"/>
+      <c r="G9" s="32"/>
+      <c r="H9" s="32"/>
+      <c r="I9" s="32"/>
+      <c r="J9" s="32"/>
+      <c r="K9" s="32"/>
+      <c r="L9" s="32"/>
+      <c r="M9" s="32"/>
+      <c r="N9" s="32"/>
+      <c r="O9" s="32"/>
+      <c r="P9" s="32"/>
+      <c r="Q9" s="32"/>
+      <c r="R9" s="32"/>
+      <c r="S9" s="32"/>
+      <c r="T9" s="32"/>
+      <c r="U9" s="32"/>
+      <c r="V9" s="32"/>
+      <c r="W9" s="32"/>
+      <c r="X9" s="32"/>
+      <c r="Y9" s="32"/>
+      <c r="Z9" s="32"/>
     </row>
     <row r="10" spans="1:26" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="16"/>
-      <c r="B10" s="16"/>
-      <c r="C10" s="16"/>
-      <c r="D10" s="16"/>
-      <c r="E10" s="16"/>
-      <c r="F10" s="16"/>
-      <c r="G10" s="16"/>
-      <c r="H10" s="16"/>
-      <c r="I10" s="16"/>
-      <c r="J10" s="16"/>
-      <c r="K10" s="16"/>
-      <c r="L10" s="16"/>
-      <c r="M10" s="16"/>
-      <c r="N10" s="16"/>
-      <c r="O10" s="16"/>
-      <c r="P10" s="16"/>
-      <c r="Q10" s="16"/>
-      <c r="R10" s="16"/>
-      <c r="S10" s="16"/>
-      <c r="T10" s="16"/>
-      <c r="U10" s="16"/>
-      <c r="V10" s="16"/>
-      <c r="W10" s="16"/>
-      <c r="X10" s="16"/>
-      <c r="Y10" s="16"/>
-      <c r="Z10" s="16"/>
+      <c r="A10" s="32"/>
+      <c r="B10" s="32"/>
+      <c r="C10" s="32"/>
+      <c r="D10" s="32"/>
+      <c r="E10" s="32"/>
+      <c r="F10" s="32"/>
+      <c r="G10" s="32"/>
+      <c r="H10" s="32"/>
+      <c r="I10" s="32"/>
+      <c r="J10" s="32"/>
+      <c r="K10" s="32"/>
+      <c r="L10" s="32"/>
+      <c r="M10" s="32"/>
+      <c r="N10" s="32"/>
+      <c r="O10" s="32"/>
+      <c r="P10" s="32"/>
+      <c r="Q10" s="32"/>
+      <c r="R10" s="32"/>
+      <c r="S10" s="32"/>
+      <c r="T10" s="32"/>
+      <c r="U10" s="32"/>
+      <c r="V10" s="32"/>
+      <c r="W10" s="32"/>
+      <c r="X10" s="32"/>
+      <c r="Y10" s="32"/>
+      <c r="Z10" s="32"/>
     </row>
     <row r="11" spans="1:26" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="16"/>
-      <c r="B11" s="16"/>
-      <c r="C11" s="16"/>
-      <c r="D11" s="16"/>
-      <c r="E11" s="16"/>
-      <c r="F11" s="16"/>
-      <c r="G11" s="16"/>
-      <c r="H11" s="16"/>
-      <c r="I11" s="16"/>
-      <c r="J11" s="16"/>
-      <c r="K11" s="16"/>
-      <c r="L11" s="16"/>
-      <c r="M11" s="16"/>
-      <c r="N11" s="16"/>
-      <c r="O11" s="16"/>
-      <c r="P11" s="16"/>
-      <c r="Q11" s="16"/>
-      <c r="R11" s="16"/>
-      <c r="S11" s="16"/>
-      <c r="T11" s="16"/>
-      <c r="U11" s="16"/>
-      <c r="V11" s="16"/>
-      <c r="W11" s="16"/>
-      <c r="X11" s="16"/>
-      <c r="Y11" s="16"/>
-      <c r="Z11" s="16"/>
+      <c r="A11" s="32"/>
+      <c r="B11" s="32"/>
+      <c r="C11" s="32"/>
+      <c r="D11" s="32"/>
+      <c r="E11" s="32"/>
+      <c r="F11" s="32"/>
+      <c r="G11" s="32"/>
+      <c r="H11" s="32"/>
+      <c r="I11" s="32"/>
+      <c r="J11" s="32"/>
+      <c r="K11" s="32"/>
+      <c r="L11" s="32"/>
+      <c r="M11" s="32"/>
+      <c r="N11" s="32"/>
+      <c r="O11" s="32"/>
+      <c r="P11" s="32"/>
+      <c r="Q11" s="32"/>
+      <c r="R11" s="32"/>
+      <c r="S11" s="32"/>
+      <c r="T11" s="32"/>
+      <c r="U11" s="32"/>
+      <c r="V11" s="32"/>
+      <c r="W11" s="32"/>
+      <c r="X11" s="32"/>
+      <c r="Y11" s="32"/>
+      <c r="Z11" s="32"/>
     </row>
     <row r="14" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="G14" s="17" t="s">
+      <c r="G14" s="29" t="s">
         <v>0</v>
       </c>
-      <c r="H14" s="18"/>
-      <c r="I14" s="19"/>
-      <c r="K14" s="20" t="s">
+      <c r="H14" s="30"/>
+      <c r="I14" s="31"/>
+      <c r="K14" s="21" t="s">
         <v>26</v>
       </c>
-      <c r="L14" s="21"/>
-      <c r="M14" s="21"/>
-      <c r="N14" s="21"/>
-      <c r="O14" s="21"/>
-      <c r="P14" s="21"/>
-      <c r="Q14" s="21"/>
-      <c r="R14" s="21"/>
-      <c r="S14" s="21"/>
-      <c r="T14" s="21"/>
-      <c r="U14" s="21"/>
-      <c r="V14" s="22"/>
+      <c r="L14" s="22"/>
+      <c r="M14" s="22"/>
+      <c r="N14" s="22"/>
+      <c r="O14" s="22"/>
+      <c r="P14" s="22"/>
+      <c r="Q14" s="22"/>
+      <c r="R14" s="22"/>
+      <c r="S14" s="22"/>
+      <c r="T14" s="22"/>
+      <c r="U14" s="22"/>
+      <c r="V14" s="23"/>
     </row>
     <row r="15" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="G15" s="17" t="s">
+      <c r="G15" s="29" t="s">
         <v>1</v>
       </c>
-      <c r="H15" s="18"/>
-      <c r="I15" s="19"/>
-      <c r="K15" s="23" t="s">
+      <c r="H15" s="30"/>
+      <c r="I15" s="31"/>
+      <c r="K15" s="33" t="s">
         <v>27</v>
       </c>
-      <c r="L15" s="21"/>
-      <c r="M15" s="21"/>
-      <c r="N15" s="21"/>
-      <c r="O15" s="21"/>
-      <c r="P15" s="21"/>
-      <c r="Q15" s="21"/>
-      <c r="R15" s="21"/>
-      <c r="S15" s="21"/>
-      <c r="T15" s="21"/>
-      <c r="U15" s="21"/>
-      <c r="V15" s="22"/>
+      <c r="L15" s="22"/>
+      <c r="M15" s="22"/>
+      <c r="N15" s="22"/>
+      <c r="O15" s="22"/>
+      <c r="P15" s="22"/>
+      <c r="Q15" s="22"/>
+      <c r="R15" s="22"/>
+      <c r="S15" s="22"/>
+      <c r="T15" s="22"/>
+      <c r="U15" s="22"/>
+      <c r="V15" s="23"/>
     </row>
     <row r="16" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="G16" s="17" t="s">
+      <c r="G16" s="29" t="s">
         <v>2</v>
       </c>
-      <c r="H16" s="18"/>
-      <c r="I16" s="19"/>
+      <c r="H16" s="30"/>
+      <c r="I16" s="31"/>
       <c r="K16" s="24" t="s">
         <v>7</v>
       </c>
@@ -2162,53 +2159,53 @@
       <c r="V16" s="26"/>
     </row>
     <row r="19" spans="7:22" x14ac:dyDescent="0.25">
-      <c r="G19" s="17" t="s">
+      <c r="G19" s="29" t="s">
         <v>3</v>
       </c>
-      <c r="H19" s="18"/>
-      <c r="I19" s="19"/>
-      <c r="K19" s="20" t="s">
+      <c r="H19" s="30"/>
+      <c r="I19" s="31"/>
+      <c r="K19" s="21" t="s">
         <v>8</v>
       </c>
-      <c r="L19" s="21"/>
-      <c r="M19" s="21"/>
-      <c r="N19" s="21"/>
-      <c r="O19" s="21"/>
-      <c r="P19" s="21"/>
-      <c r="Q19" s="21"/>
-      <c r="R19" s="21"/>
-      <c r="S19" s="21"/>
-      <c r="T19" s="21"/>
-      <c r="U19" s="21"/>
-      <c r="V19" s="22"/>
+      <c r="L19" s="22"/>
+      <c r="M19" s="22"/>
+      <c r="N19" s="22"/>
+      <c r="O19" s="22"/>
+      <c r="P19" s="22"/>
+      <c r="Q19" s="22"/>
+      <c r="R19" s="22"/>
+      <c r="S19" s="22"/>
+      <c r="T19" s="22"/>
+      <c r="U19" s="22"/>
+      <c r="V19" s="23"/>
     </row>
     <row r="20" spans="7:22" x14ac:dyDescent="0.25">
-      <c r="G20" s="17" t="s">
+      <c r="G20" s="29" t="s">
         <v>4</v>
       </c>
-      <c r="H20" s="18"/>
-      <c r="I20" s="19"/>
-      <c r="K20" s="20" t="s">
+      <c r="H20" s="30"/>
+      <c r="I20" s="31"/>
+      <c r="K20" s="21" t="s">
         <v>9</v>
       </c>
-      <c r="L20" s="21"/>
-      <c r="M20" s="21"/>
-      <c r="N20" s="21"/>
-      <c r="O20" s="21"/>
-      <c r="P20" s="21"/>
-      <c r="Q20" s="21"/>
-      <c r="R20" s="21"/>
-      <c r="S20" s="21"/>
-      <c r="T20" s="21"/>
-      <c r="U20" s="21"/>
-      <c r="V20" s="22"/>
+      <c r="L20" s="22"/>
+      <c r="M20" s="22"/>
+      <c r="N20" s="22"/>
+      <c r="O20" s="22"/>
+      <c r="P20" s="22"/>
+      <c r="Q20" s="22"/>
+      <c r="R20" s="22"/>
+      <c r="S20" s="22"/>
+      <c r="T20" s="22"/>
+      <c r="U20" s="22"/>
+      <c r="V20" s="23"/>
     </row>
     <row r="21" spans="7:22" x14ac:dyDescent="0.25">
-      <c r="G21" s="17" t="s">
+      <c r="G21" s="29" t="s">
         <v>5</v>
       </c>
-      <c r="H21" s="18"/>
-      <c r="I21" s="19"/>
+      <c r="H21" s="30"/>
+      <c r="I21" s="31"/>
       <c r="K21" s="24" t="s">
         <v>10</v>
       </c>
@@ -2225,11 +2222,11 @@
       <c r="V21" s="26"/>
     </row>
     <row r="24" spans="7:22" x14ac:dyDescent="0.25">
-      <c r="G24" s="17" t="s">
+      <c r="G24" s="29" t="s">
         <v>6</v>
       </c>
-      <c r="H24" s="18"/>
-      <c r="I24" s="19"/>
+      <c r="H24" s="30"/>
+      <c r="I24" s="31"/>
       <c r="K24" s="27">
         <v>45439</v>
       </c>
@@ -2247,6 +2244,13 @@
     </row>
   </sheetData>
   <mergeCells count="15">
+    <mergeCell ref="A1:Z11"/>
+    <mergeCell ref="G14:I14"/>
+    <mergeCell ref="K14:V14"/>
+    <mergeCell ref="G15:I15"/>
+    <mergeCell ref="G16:I16"/>
+    <mergeCell ref="K15:V15"/>
+    <mergeCell ref="K16:V16"/>
     <mergeCell ref="K19:V19"/>
     <mergeCell ref="K20:V20"/>
     <mergeCell ref="K21:V21"/>
@@ -2255,13 +2259,6 @@
     <mergeCell ref="G20:I20"/>
     <mergeCell ref="G21:I21"/>
     <mergeCell ref="G24:I24"/>
-    <mergeCell ref="A1:Z11"/>
-    <mergeCell ref="G14:I14"/>
-    <mergeCell ref="K14:V14"/>
-    <mergeCell ref="G15:I15"/>
-    <mergeCell ref="G16:I16"/>
-    <mergeCell ref="K15:V15"/>
-    <mergeCell ref="K16:V16"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="K15" r:id="rId1" xr:uid="{B39E7FA7-0077-4592-BE7E-C6FE950055E9}"/>
@@ -2275,7 +2272,7 @@
   <dimension ref="A1:I21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C23" sqref="C23"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2819,8 +2816,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E2C1E1C6-748F-4782-83CA-6948B67C52D3}">
   <dimension ref="A1:H98"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="H24" sqref="H24"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2862,16 +2859,16 @@
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2" s="29" t="s">
+      <c r="A2" s="34" t="s">
         <v>50</v>
       </c>
-      <c r="B2" s="30"/>
-      <c r="C2" s="30"/>
-      <c r="D2" s="30"/>
-      <c r="E2" s="30"/>
-      <c r="F2" s="30"/>
-      <c r="G2" s="30"/>
-      <c r="H2" s="31"/>
+      <c r="B2" s="35"/>
+      <c r="C2" s="35"/>
+      <c r="D2" s="35"/>
+      <c r="E2" s="35"/>
+      <c r="F2" s="35"/>
+      <c r="G2" s="35"/>
+      <c r="H2" s="36"/>
     </row>
     <row r="3" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A3" s="15">
@@ -2916,7 +2913,9 @@
       <c r="F4" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="G4" s="5"/>
+      <c r="G4" s="5" t="s">
+        <v>19</v>
+      </c>
       <c r="H4" s="3"/>
     </row>
     <row r="5" spans="1:8" ht="120" x14ac:dyDescent="0.25">
@@ -2938,7 +2937,9 @@
       <c r="F5" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="G5" s="5"/>
+      <c r="G5" s="5" t="s">
+        <v>19</v>
+      </c>
       <c r="H5" s="3"/>
     </row>
     <row r="6" spans="1:8" ht="120" x14ac:dyDescent="0.25">
@@ -2960,7 +2961,9 @@
       <c r="F6" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="G6" s="5"/>
+      <c r="G6" s="5" t="s">
+        <v>19</v>
+      </c>
       <c r="H6" s="3"/>
     </row>
     <row r="7" spans="1:8" ht="120" x14ac:dyDescent="0.25">
@@ -2982,7 +2985,9 @@
       <c r="F7" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="G7" s="5"/>
+      <c r="G7" s="5" t="s">
+        <v>19</v>
+      </c>
       <c r="H7" s="3"/>
     </row>
     <row r="8" spans="1:8" ht="120" x14ac:dyDescent="0.25">
@@ -3004,7 +3009,9 @@
       <c r="F8" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="G8" s="5"/>
+      <c r="G8" s="5" t="s">
+        <v>19</v>
+      </c>
       <c r="H8" s="3"/>
     </row>
     <row r="9" spans="1:8" ht="120" x14ac:dyDescent="0.25">
@@ -3023,7 +3030,7 @@
       <c r="E9" s="4" t="s">
         <v>199</v>
       </c>
-      <c r="F9" s="37" t="s">
+      <c r="F9" s="20" t="s">
         <v>195</v>
       </c>
       <c r="G9" s="5" t="s">
@@ -3052,7 +3059,9 @@
       <c r="F10" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="G10" s="5"/>
+      <c r="G10" s="5" t="s">
+        <v>19</v>
+      </c>
       <c r="H10" s="3"/>
     </row>
     <row r="11" spans="1:8" ht="45" x14ac:dyDescent="0.25">
@@ -3074,7 +3083,9 @@
       <c r="F11" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="G11" s="5"/>
+      <c r="G11" s="5" t="s">
+        <v>19</v>
+      </c>
       <c r="H11" s="3"/>
     </row>
     <row r="12" spans="1:8" ht="135" x14ac:dyDescent="0.25">
@@ -3096,76 +3107,82 @@
       <c r="F12" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="G12" s="5"/>
+      <c r="G12" s="5" t="s">
+        <v>19</v>
+      </c>
       <c r="H12" s="3"/>
     </row>
     <row r="13" spans="1:8" ht="120" x14ac:dyDescent="0.25">
-      <c r="A13" s="32">
+      <c r="A13" s="16">
         <v>11</v>
       </c>
-      <c r="B13" s="33" t="s">
+      <c r="B13" s="17" t="s">
         <v>127</v>
       </c>
-      <c r="C13" s="33" t="s">
+      <c r="C13" s="17" t="s">
         <v>78</v>
       </c>
-      <c r="D13" s="33" t="s">
+      <c r="D13" s="17" t="s">
         <v>79</v>
       </c>
-      <c r="E13" s="33" t="s">
+      <c r="E13" s="17" t="s">
         <v>80</v>
       </c>
       <c r="F13" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="G13" s="34"/>
-      <c r="H13" s="32"/>
+      <c r="G13" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="H13" s="16"/>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A14" s="29" t="s">
+      <c r="A14" s="34" t="s">
         <v>51</v>
       </c>
-      <c r="B14" s="30"/>
-      <c r="C14" s="30"/>
-      <c r="D14" s="30"/>
-      <c r="E14" s="30"/>
-      <c r="F14" s="30"/>
-      <c r="G14" s="30"/>
-      <c r="H14" s="31"/>
+      <c r="B14" s="35"/>
+      <c r="C14" s="35"/>
+      <c r="D14" s="35"/>
+      <c r="E14" s="35"/>
+      <c r="F14" s="35"/>
+      <c r="G14" s="35"/>
+      <c r="H14" s="36"/>
     </row>
     <row r="15" spans="1:8" ht="120" x14ac:dyDescent="0.25">
       <c r="A15" s="15">
         <v>12</v>
       </c>
-      <c r="B15" s="35" t="s">
+      <c r="B15" s="18" t="s">
         <v>87</v>
       </c>
-      <c r="C15" s="35" t="s">
+      <c r="C15" s="18" t="s">
         <v>88</v>
       </c>
-      <c r="D15" s="35" t="s">
+      <c r="D15" s="18" t="s">
         <v>89</v>
       </c>
-      <c r="E15" s="35" t="s">
+      <c r="E15" s="18" t="s">
         <v>90</v>
       </c>
       <c r="F15" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="G15" s="36"/>
+      <c r="G15" s="5" t="s">
+        <v>19</v>
+      </c>
       <c r="H15" s="15"/>
     </row>
     <row r="16" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A16" s="15">
         <v>13</v>
       </c>
-      <c r="B16" s="35" t="s">
+      <c r="B16" s="18" t="s">
         <v>92</v>
       </c>
-      <c r="C16" s="35" t="s">
+      <c r="C16" s="18" t="s">
         <v>91</v>
       </c>
-      <c r="D16" s="35" t="s">
+      <c r="D16" s="18" t="s">
         <v>93</v>
       </c>
       <c r="E16" s="15" t="s">
@@ -3174,7 +3191,9 @@
       <c r="F16" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="G16" s="36"/>
+      <c r="G16" s="5" t="s">
+        <v>19</v>
+      </c>
       <c r="H16" s="15"/>
     </row>
     <row r="17" spans="1:8" ht="60" x14ac:dyDescent="0.25">
@@ -3196,7 +3215,9 @@
       <c r="F17" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="G17" s="36"/>
+      <c r="G17" s="5" t="s">
+        <v>19</v>
+      </c>
       <c r="H17" s="15"/>
     </row>
     <row r="18" spans="1:8" ht="60" x14ac:dyDescent="0.25">
@@ -3218,7 +3239,9 @@
       <c r="F18" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="G18" s="36"/>
+      <c r="G18" s="5" t="s">
+        <v>19</v>
+      </c>
       <c r="H18" s="15"/>
     </row>
     <row r="19" spans="1:8" ht="60" x14ac:dyDescent="0.25">
@@ -3240,7 +3263,9 @@
       <c r="F19" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="G19" s="36"/>
+      <c r="G19" s="5" t="s">
+        <v>19</v>
+      </c>
       <c r="H19" s="15"/>
     </row>
     <row r="20" spans="1:8" ht="60" x14ac:dyDescent="0.25">
@@ -3262,7 +3287,9 @@
       <c r="F20" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="G20" s="36"/>
+      <c r="G20" s="5" t="s">
+        <v>19</v>
+      </c>
       <c r="H20" s="15"/>
     </row>
     <row r="21" spans="1:8" ht="60" x14ac:dyDescent="0.25">
@@ -3284,7 +3311,9 @@
       <c r="F21" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="G21" s="36"/>
+      <c r="G21" s="5" t="s">
+        <v>19</v>
+      </c>
       <c r="H21" s="15"/>
     </row>
     <row r="22" spans="1:8" ht="60" x14ac:dyDescent="0.25">
@@ -3306,7 +3335,9 @@
       <c r="F22" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="G22" s="36"/>
+      <c r="G22" s="5" t="s">
+        <v>19</v>
+      </c>
       <c r="H22" s="15"/>
     </row>
     <row r="23" spans="1:8" ht="60" x14ac:dyDescent="0.25">
@@ -3325,10 +3356,12 @@
       <c r="E23" s="4" t="s">
         <v>198</v>
       </c>
-      <c r="F23" s="37" t="s">
+      <c r="F23" s="20" t="s">
         <v>195</v>
       </c>
-      <c r="G23" s="36"/>
+      <c r="G23" s="19" t="s">
+        <v>200</v>
+      </c>
       <c r="H23" s="3" t="s">
         <v>202</v>
       </c>
@@ -3352,42 +3385,46 @@
       <c r="F24" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="G24" s="36"/>
+      <c r="G24" s="5" t="s">
+        <v>19</v>
+      </c>
       <c r="H24" s="15"/>
     </row>
     <row r="25" spans="1:8" ht="120" x14ac:dyDescent="0.25">
-      <c r="A25" s="32">
+      <c r="A25" s="16">
         <v>22</v>
       </c>
-      <c r="B25" s="33" t="s">
+      <c r="B25" s="17" t="s">
         <v>115</v>
       </c>
-      <c r="C25" s="33" t="s">
+      <c r="C25" s="17" t="s">
         <v>116</v>
       </c>
-      <c r="D25" s="33" t="s">
+      <c r="D25" s="17" t="s">
         <v>118</v>
       </c>
-      <c r="E25" s="33" t="s">
+      <c r="E25" s="17" t="s">
         <v>119</v>
       </c>
       <c r="F25" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="G25" s="36"/>
+      <c r="G25" s="5" t="s">
+        <v>19</v>
+      </c>
       <c r="H25" s="15"/>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A26" s="29" t="s">
+      <c r="A26" s="34" t="s">
         <v>67</v>
       </c>
-      <c r="B26" s="30"/>
-      <c r="C26" s="30"/>
-      <c r="D26" s="30"/>
-      <c r="E26" s="30"/>
-      <c r="F26" s="30"/>
-      <c r="G26" s="30"/>
-      <c r="H26" s="31"/>
+      <c r="B26" s="35"/>
+      <c r="C26" s="35"/>
+      <c r="D26" s="35"/>
+      <c r="E26" s="35"/>
+      <c r="F26" s="35"/>
+      <c r="G26" s="35"/>
+      <c r="H26" s="36"/>
     </row>
     <row r="27" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A27" s="3">
@@ -3408,7 +3445,9 @@
       <c r="F27" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="G27" s="5"/>
+      <c r="G27" s="5" t="s">
+        <v>19</v>
+      </c>
       <c r="H27" s="3"/>
     </row>
     <row r="28" spans="1:8" ht="45" x14ac:dyDescent="0.25">
@@ -3430,42 +3469,46 @@
       <c r="F28" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="G28" s="5"/>
+      <c r="G28" s="5" t="s">
+        <v>19</v>
+      </c>
       <c r="H28" s="3"/>
     </row>
     <row r="29" spans="1:8" ht="45" x14ac:dyDescent="0.25">
-      <c r="A29" s="32">
+      <c r="A29" s="16">
         <v>25</v>
       </c>
-      <c r="B29" s="32" t="s">
+      <c r="B29" s="16" t="s">
         <v>136</v>
       </c>
-      <c r="C29" s="33" t="s">
+      <c r="C29" s="17" t="s">
         <v>137</v>
       </c>
-      <c r="D29" s="33" t="s">
+      <c r="D29" s="17" t="s">
         <v>139</v>
       </c>
-      <c r="E29" s="33" t="s">
+      <c r="E29" s="17" t="s">
         <v>138</v>
       </c>
       <c r="F29" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="G29" s="34"/>
-      <c r="H29" s="32"/>
+      <c r="G29" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="H29" s="16"/>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A30" s="29" t="s">
+      <c r="A30" s="34" t="s">
         <v>61</v>
       </c>
-      <c r="B30" s="30"/>
-      <c r="C30" s="30"/>
-      <c r="D30" s="30"/>
-      <c r="E30" s="30"/>
-      <c r="F30" s="30"/>
-      <c r="G30" s="30"/>
-      <c r="H30" s="31"/>
+      <c r="B30" s="35"/>
+      <c r="C30" s="35"/>
+      <c r="D30" s="35"/>
+      <c r="E30" s="35"/>
+      <c r="F30" s="35"/>
+      <c r="G30" s="35"/>
+      <c r="H30" s="36"/>
     </row>
     <row r="31" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A31" s="3">
@@ -3486,7 +3529,9 @@
       <c r="F31" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="G31" s="5"/>
+      <c r="G31" s="5" t="s">
+        <v>19</v>
+      </c>
       <c r="H31" s="3"/>
     </row>
     <row r="32" spans="1:8" ht="45" x14ac:dyDescent="0.25">
@@ -3508,7 +3553,9 @@
       <c r="F32" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="G32" s="5"/>
+      <c r="G32" s="5" t="s">
+        <v>19</v>
+      </c>
       <c r="H32" s="3"/>
     </row>
     <row r="33" spans="1:8" ht="45" x14ac:dyDescent="0.25">
@@ -3530,7 +3577,9 @@
       <c r="F33" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="G33" s="5"/>
+      <c r="G33" s="5" t="s">
+        <v>19</v>
+      </c>
       <c r="H33" s="3"/>
     </row>
     <row r="34" spans="1:8" ht="45" x14ac:dyDescent="0.25">
@@ -3552,7 +3601,9 @@
       <c r="F34" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="G34" s="5"/>
+      <c r="G34" s="5" t="s">
+        <v>19</v>
+      </c>
       <c r="H34" s="3"/>
     </row>
     <row r="35" spans="1:8" ht="45" x14ac:dyDescent="0.25">
@@ -3574,7 +3625,9 @@
       <c r="F35" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="G35" s="5"/>
+      <c r="G35" s="5" t="s">
+        <v>19</v>
+      </c>
       <c r="H35" s="3"/>
     </row>
     <row r="36" spans="1:8" ht="45" x14ac:dyDescent="0.25">
@@ -3596,20 +3649,22 @@
       <c r="F36" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="G36" s="5"/>
+      <c r="G36" s="5" t="s">
+        <v>19</v>
+      </c>
       <c r="H36" s="3"/>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A37" s="29" t="s">
+      <c r="A37" s="34" t="s">
         <v>68</v>
       </c>
-      <c r="B37" s="30"/>
-      <c r="C37" s="30"/>
-      <c r="D37" s="30"/>
-      <c r="E37" s="30"/>
-      <c r="F37" s="30"/>
-      <c r="G37" s="30"/>
-      <c r="H37" s="31"/>
+      <c r="B37" s="35"/>
+      <c r="C37" s="35"/>
+      <c r="D37" s="35"/>
+      <c r="E37" s="35"/>
+      <c r="F37" s="35"/>
+      <c r="G37" s="35"/>
+      <c r="H37" s="36"/>
     </row>
     <row r="38" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A38" s="3">
@@ -3630,7 +3685,9 @@
       <c r="F38" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="G38" s="5"/>
+      <c r="G38" s="5" t="s">
+        <v>19</v>
+      </c>
       <c r="H38" s="3"/>
     </row>
     <row r="39" spans="1:8" ht="30" x14ac:dyDescent="0.25">
@@ -3652,7 +3709,9 @@
       <c r="F39" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="G39" s="5"/>
+      <c r="G39" s="5" t="s">
+        <v>19</v>
+      </c>
       <c r="H39" s="3"/>
     </row>
     <row r="40" spans="1:8" ht="30" x14ac:dyDescent="0.25">
@@ -3674,20 +3733,22 @@
       <c r="F40" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="G40" s="5"/>
+      <c r="G40" s="5" t="s">
+        <v>19</v>
+      </c>
       <c r="H40" s="3"/>
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A41" s="29" t="s">
+      <c r="A41" s="34" t="s">
         <v>69</v>
       </c>
-      <c r="B41" s="30"/>
-      <c r="C41" s="30"/>
-      <c r="D41" s="30"/>
-      <c r="E41" s="30"/>
-      <c r="F41" s="30"/>
-      <c r="G41" s="30"/>
-      <c r="H41" s="31"/>
+      <c r="B41" s="35"/>
+      <c r="C41" s="35"/>
+      <c r="D41" s="35"/>
+      <c r="E41" s="35"/>
+      <c r="F41" s="35"/>
+      <c r="G41" s="35"/>
+      <c r="H41" s="36"/>
     </row>
     <row r="42" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A42" s="3">
@@ -3708,7 +3769,9 @@
       <c r="F42" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="G42" s="5"/>
+      <c r="G42" s="5" t="s">
+        <v>19</v>
+      </c>
       <c r="H42" s="3"/>
     </row>
     <row r="43" spans="1:8" ht="30" x14ac:dyDescent="0.25">
@@ -3730,7 +3793,9 @@
       <c r="F43" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="G43" s="5"/>
+      <c r="G43" s="5" t="s">
+        <v>19</v>
+      </c>
       <c r="H43" s="3"/>
     </row>
     <row r="44" spans="1:8" ht="30" x14ac:dyDescent="0.25">
@@ -3752,7 +3817,9 @@
       <c r="F44" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="G44" s="5"/>
+      <c r="G44" s="5" t="s">
+        <v>19</v>
+      </c>
       <c r="H44" s="3"/>
     </row>
     <row r="45" spans="1:8" ht="30" x14ac:dyDescent="0.25">
@@ -3774,7 +3841,9 @@
       <c r="F45" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="G45" s="5"/>
+      <c r="G45" s="5" t="s">
+        <v>19</v>
+      </c>
       <c r="H45" s="3"/>
     </row>
     <row r="46" spans="1:8" ht="30" x14ac:dyDescent="0.25">
@@ -3796,7 +3865,9 @@
       <c r="F46" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="G46" s="5"/>
+      <c r="G46" s="5" t="s">
+        <v>19</v>
+      </c>
       <c r="H46" s="3"/>
     </row>
     <row r="47" spans="1:8" x14ac:dyDescent="0.25">
@@ -4332,7 +4403,7 @@
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G3" xr:uid="{9E7A5853-1C00-445C-9290-798981E423AE}">
       <formula1>"A - High, B - Medium, C - Low, None"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G42:G98 G27:G29 G31:G36 G38:G40 G4:G13 G15:G25" xr:uid="{1D89D116-AAC3-4E50-911F-ACA0B7F5AAEC}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G38:G40 G15:G25 G27:G29 G31:G36 G4:G13 G42:G98" xr:uid="{1D89D116-AAC3-4E50-911F-ACA0B7F5AAEC}">
       <formula1>"A- High, B - Medium, C - Low, None"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>